<commit_message>
C06.00.08 - docs(src): Model map added
Map of the physical model with reference axes and actuator directions
added
</commit_message>
<xml_diff>
--- a/hardware/boards/warehouse_v2/docs/Documentation_WH.xlsx
+++ b/hardware/boards/warehouse_v2/docs/Documentation_WH.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\Basurero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03DC6548-B543-4143-86DA-19589620C89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A96D80-0DCA-495D-BE11-589671D4C7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{658C6C44-180A-4413-9118-4B5F379EEF28}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{658C6C44-180A-4413-9118-4B5F379EEF28}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
     <sheet name="Registers" sheetId="2" r:id="rId2"/>
     <sheet name="Error List" sheetId="4" r:id="rId3"/>
     <sheet name="SPI Protocol" sheetId="3" r:id="rId4"/>
+    <sheet name="Map" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="353">
   <si>
     <t>Signal Name</t>
   </si>
@@ -819,12 +820,6 @@
   </si>
   <si>
     <t>Data</t>
-  </si>
-  <si>
-    <t>Dir</t>
-  </si>
-  <si>
-    <t>Enb</t>
   </si>
   <si>
     <t>Stall</t>
@@ -1111,6 +1106,78 @@
   </si>
   <si>
     <t>Dir1</t>
+  </si>
+  <si>
+    <t>Physical model reference map</t>
+  </si>
+  <si>
+    <t>Status LEDs</t>
+  </si>
+  <si>
+    <t>Model connectors</t>
+  </si>
+  <si>
+    <t>Stepper0</t>
+  </si>
+  <si>
+    <t>Stepper1</t>
+  </si>
+  <si>
+    <t>DC_Motor</t>
+  </si>
+  <si>
+    <t>X-Axis</t>
+  </si>
+  <si>
+    <t>Y-Axis</t>
+  </si>
+  <si>
+    <t>Z-Axis</t>
+  </si>
+  <si>
+    <t>Actuation Map</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>x_neg | left</t>
+  </si>
+  <si>
+    <t>Stepper0 -&gt; Dir0</t>
+  </si>
+  <si>
+    <t>x_pos | right</t>
+  </si>
+  <si>
+    <t>Stepper0 -&gt; Dir1</t>
+  </si>
+  <si>
+    <t>y_neg | Outside</t>
+  </si>
+  <si>
+    <t>DC -&gt; Inside</t>
+  </si>
+  <si>
+    <t>DC -&gt; Outside</t>
+  </si>
+  <si>
+    <t>y_pos | Inside</t>
+  </si>
+  <si>
+    <t>z_neg | bottom</t>
+  </si>
+  <si>
+    <t>Stepper1 -&gt; Dir0</t>
+  </si>
+  <si>
+    <t>z_pos | top</t>
+  </si>
+  <si>
+    <t>Stepper1 -&gt; Dir1</t>
   </si>
 </sst>
 </file>
@@ -1199,15 +1266,51 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="53">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -1877,12 +1980,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1997,6 +2206,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2033,18 +2248,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2106,6 +2321,60 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2124,6 +2393,179 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7AA7801-B353-96B7-C14D-227C09B73BA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="4229100"/>
+          <a:ext cx="640080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{887A14A8-3051-447C-9574-C50D8CF8C43B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="906780" y="3916680"/>
+          <a:ext cx="640080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21C621C8-C79F-45D1-8774-4512A008FC10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="845820" y="4221480"/>
+          <a:ext cx="381000" cy="236220"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2448,30 +2890,30 @@
   <sheetData>
     <row r="1" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="69" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="65"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="71"/>
     </row>
     <row r="3" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="60" t="s">
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="66" t="s">
         <v>149</v>
       </c>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="2:9" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="30" t="s">
@@ -3740,8 +4182,8 @@
   </sheetPr>
   <dimension ref="B2:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:M24"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3758,26 +4200,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="75" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="76" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="70"/>
+      <c r="C3" s="76"/>
       <c r="D3" s="1">
         <v>1</v>
       </c>
@@ -3792,10 +4234,10 @@
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="76" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="70"/>
+      <c r="C4" s="76"/>
       <c r="D4" s="2" t="s">
         <v>155</v>
       </c>
@@ -3810,10 +4252,10 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="76" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="70"/>
+      <c r="C5" s="76"/>
       <c r="D5" s="3" t="s">
         <v>156</v>
       </c>
@@ -3828,34 +4270,34 @@
       <c r="M5" s="1"/>
     </row>
     <row r="7" spans="2:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="77" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
     </row>
     <row r="9" spans="2:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="13"/>
@@ -4149,16 +4591,16 @@
       <c r="E19" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F19" s="68" t="s">
+      <c r="F19" s="74" t="s">
         <v>247</v>
       </c>
-      <c r="G19" s="68"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="68"/>
-      <c r="M19" s="66"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="74"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="74"/>
+      <c r="L19" s="74"/>
+      <c r="M19" s="72"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="20" t="s">
@@ -4173,16 +4615,16 @@
       <c r="E20" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F20" s="68" t="s">
+      <c r="F20" s="74" t="s">
         <v>250</v>
       </c>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="68"/>
-      <c r="L20" s="68"/>
-      <c r="M20" s="66"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="74"/>
+      <c r="J20" s="74"/>
+      <c r="K20" s="74"/>
+      <c r="L20" s="74"/>
+      <c r="M20" s="72"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
@@ -4197,16 +4639,16 @@
       <c r="E21" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F21" s="68" t="s">
+      <c r="F21" s="74" t="s">
         <v>248</v>
       </c>
-      <c r="G21" s="68"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="68"/>
-      <c r="K21" s="68"/>
-      <c r="L21" s="68"/>
-      <c r="M21" s="66"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="74"/>
+      <c r="L21" s="74"/>
+      <c r="M21" s="72"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
@@ -4221,16 +4663,16 @@
       <c r="E22" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F22" s="68" t="s">
+      <c r="F22" s="74" t="s">
         <v>249</v>
       </c>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="68"/>
-      <c r="L22" s="68"/>
-      <c r="M22" s="66"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="74"/>
+      <c r="M22" s="72"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="20" t="s">
@@ -4246,20 +4688,20 @@
         <v>221</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
       <c r="J23" s="23"/>
       <c r="K23" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="L23" s="23" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="M23" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
@@ -4275,16 +4717,16 @@
       <c r="E24" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F24" s="68" t="s">
+      <c r="F24" s="74" t="s">
         <v>251</v>
       </c>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="66"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="74"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="72"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="20" t="s">
@@ -4299,16 +4741,16 @@
       <c r="E25" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F25" s="66" t="s">
-        <v>294</v>
-      </c>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="67"/>
-      <c r="L25" s="67"/>
-      <c r="M25" s="67"/>
+      <c r="F25" s="72" t="s">
+        <v>292</v>
+      </c>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="73"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="20" t="s">
@@ -4323,16 +4765,16 @@
       <c r="E26" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="F26" s="68" t="s">
+      <c r="F26" s="74" t="s">
         <v>252</v>
       </c>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="68"/>
-      <c r="L26" s="68"/>
-      <c r="M26" s="66"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="74"/>
+      <c r="M26" s="72"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="20" t="s">
@@ -4347,16 +4789,16 @@
       <c r="E27" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F27" s="68" t="s">
+      <c r="F27" s="74" t="s">
         <v>253</v>
       </c>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="68"/>
-      <c r="M27" s="66"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="74"/>
+      <c r="M27" s="72"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
@@ -4371,16 +4813,16 @@
       <c r="E28" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F28" s="66" t="s">
-        <v>328</v>
-      </c>
-      <c r="G28" s="67"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="67"/>
-      <c r="J28" s="67"/>
-      <c r="K28" s="67"/>
-      <c r="L28" s="67"/>
-      <c r="M28" s="67"/>
+      <c r="F28" s="72" t="s">
+        <v>326</v>
+      </c>
+      <c r="G28" s="73"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="73"/>
+      <c r="J28" s="73"/>
+      <c r="K28" s="73"/>
+      <c r="L28" s="73"/>
+      <c r="M28" s="73"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
@@ -4421,16 +4863,16 @@
       <c r="E30" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F30" s="68" t="s">
+      <c r="F30" s="74" t="s">
         <v>255</v>
       </c>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="68"/>
-      <c r="M30" s="66"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
+      <c r="K30" s="74"/>
+      <c r="L30" s="74"/>
+      <c r="M30" s="72"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="20" t="s">
@@ -4446,20 +4888,20 @@
         <v>221</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G31" s="23"/>
       <c r="H31" s="23"/>
       <c r="I31" s="23"/>
       <c r="J31" s="23"/>
       <c r="K31" s="23" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="L31" s="23" t="s">
-        <v>261</v>
+        <v>328</v>
       </c>
       <c r="M31" s="24" t="s">
-        <v>260</v>
+        <v>327</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
@@ -4475,16 +4917,16 @@
       <c r="E32" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F32" s="68" t="s">
+      <c r="F32" s="74" t="s">
         <v>251</v>
       </c>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="68"/>
-      <c r="L32" s="68"/>
-      <c r="M32" s="66"/>
+      <c r="G32" s="74"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="74"/>
+      <c r="K32" s="74"/>
+      <c r="L32" s="74"/>
+      <c r="M32" s="72"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="20" t="s">
@@ -4499,16 +4941,16 @@
       <c r="E33" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F33" s="68" t="s">
-        <v>294</v>
-      </c>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="68"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="68"/>
-      <c r="L33" s="68"/>
-      <c r="M33" s="66"/>
+      <c r="F33" s="74" t="s">
+        <v>292</v>
+      </c>
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="74"/>
+      <c r="M33" s="72"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="20" t="s">
@@ -4523,16 +4965,16 @@
       <c r="E34" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="F34" s="68" t="s">
+      <c r="F34" s="74" t="s">
         <v>252</v>
       </c>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="68"/>
-      <c r="K34" s="68"/>
-      <c r="L34" s="68"/>
-      <c r="M34" s="66"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="74"/>
+      <c r="K34" s="74"/>
+      <c r="L34" s="74"/>
+      <c r="M34" s="72"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="20" t="s">
@@ -4547,16 +4989,16 @@
       <c r="E35" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F35" s="68" t="s">
+      <c r="F35" s="74" t="s">
         <v>253</v>
       </c>
-      <c r="G35" s="68"/>
-      <c r="H35" s="68"/>
-      <c r="I35" s="68"/>
-      <c r="J35" s="68"/>
-      <c r="K35" s="68"/>
-      <c r="L35" s="68"/>
-      <c r="M35" s="66"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="74"/>
+      <c r="I35" s="74"/>
+      <c r="J35" s="74"/>
+      <c r="K35" s="74"/>
+      <c r="L35" s="74"/>
+      <c r="M35" s="72"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="20" t="s">
@@ -4566,7 +5008,7 @@
         <v>26</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E36" s="22" t="s">
         <v>221</v>
@@ -4575,12 +5017,12 @@
       <c r="G36" s="23"/>
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
-      <c r="J36" s="68" t="s">
+      <c r="J36" s="74" t="s">
         <v>254</v>
       </c>
-      <c r="K36" s="68"/>
-      <c r="L36" s="68"/>
-      <c r="M36" s="66"/>
+      <c r="K36" s="74"/>
+      <c r="L36" s="74"/>
+      <c r="M36" s="72"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="20" t="s">
@@ -4590,27 +5032,27 @@
         <v>27</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E37" s="22" t="s">
         <v>221</v>
       </c>
       <c r="F37" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="H37" s="80" t="s">
         <v>264</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="I37" s="80"/>
+      <c r="J37" s="80"/>
+      <c r="K37" s="80" t="s">
         <v>265</v>
       </c>
-      <c r="H37" s="72" t="s">
-        <v>266</v>
-      </c>
-      <c r="I37" s="72"/>
-      <c r="J37" s="72"/>
-      <c r="K37" s="72" t="s">
-        <v>267</v>
-      </c>
-      <c r="L37" s="72"/>
-      <c r="M37" s="73"/>
+      <c r="L37" s="80"/>
+      <c r="M37" s="81"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="20" t="s">
@@ -4620,27 +5062,27 @@
         <v>28</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E38" s="22" t="s">
         <v>221</v>
       </c>
       <c r="F38" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="H38" s="80" t="s">
         <v>264</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="I38" s="80"/>
+      <c r="J38" s="80"/>
+      <c r="K38" s="80" t="s">
         <v>265</v>
       </c>
-      <c r="H38" s="72" t="s">
-        <v>266</v>
-      </c>
-      <c r="I38" s="72"/>
-      <c r="J38" s="72"/>
-      <c r="K38" s="72" t="s">
-        <v>267</v>
-      </c>
-      <c r="L38" s="72"/>
-      <c r="M38" s="73"/>
+      <c r="L38" s="80"/>
+      <c r="M38" s="81"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="20" t="s">
@@ -4650,27 +5092,27 @@
         <v>29</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E39" s="22" t="s">
         <v>221</v>
       </c>
       <c r="F39" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="H39" s="80" t="s">
         <v>264</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="I39" s="80"/>
+      <c r="J39" s="80"/>
+      <c r="K39" s="80" t="s">
         <v>265</v>
       </c>
-      <c r="H39" s="72" t="s">
-        <v>266</v>
-      </c>
-      <c r="I39" s="72"/>
-      <c r="J39" s="72"/>
-      <c r="K39" s="72" t="s">
-        <v>267</v>
-      </c>
-      <c r="L39" s="72"/>
-      <c r="M39" s="73"/>
+      <c r="L39" s="80"/>
+      <c r="M39" s="81"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="20" t="s">
@@ -4680,27 +5122,27 @@
         <v>30</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E40" s="22" t="s">
         <v>221</v>
       </c>
       <c r="F40" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="H40" s="80" t="s">
         <v>264</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="I40" s="80"/>
+      <c r="J40" s="80"/>
+      <c r="K40" s="80" t="s">
         <v>265</v>
       </c>
-      <c r="H40" s="72" t="s">
-        <v>266</v>
-      </c>
-      <c r="I40" s="72"/>
-      <c r="J40" s="72"/>
-      <c r="K40" s="72" t="s">
-        <v>267</v>
-      </c>
-      <c r="L40" s="72"/>
-      <c r="M40" s="73"/>
+      <c r="L40" s="80"/>
+      <c r="M40" s="81"/>
     </row>
     <row r="41" spans="2:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="25" t="s">
@@ -4710,27 +5152,27 @@
         <v>31</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E41" s="28" t="s">
         <v>221</v>
       </c>
       <c r="F41" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="H41" s="78" t="s">
         <v>264</v>
       </c>
-      <c r="G41" s="8" t="s">
+      <c r="I41" s="78"/>
+      <c r="J41" s="78"/>
+      <c r="K41" s="78" t="s">
         <v>265</v>
       </c>
-      <c r="H41" s="74" t="s">
-        <v>266</v>
-      </c>
-      <c r="I41" s="74"/>
-      <c r="J41" s="74"/>
-      <c r="K41" s="74" t="s">
-        <v>267</v>
-      </c>
-      <c r="L41" s="74"/>
-      <c r="M41" s="75"/>
+      <c r="L41" s="78"/>
+      <c r="M41" s="79"/>
     </row>
     <row r="42" spans="2:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C42" s="29"/>
@@ -4739,7 +5181,12 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="F28:M28"/>
+    <mergeCell ref="F32:M32"/>
+    <mergeCell ref="F34:M34"/>
+    <mergeCell ref="F35:M35"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="K37:M37"/>
     <mergeCell ref="H41:J41"/>
     <mergeCell ref="K41:M41"/>
     <mergeCell ref="H38:J38"/>
@@ -4748,12 +5195,6 @@
     <mergeCell ref="K40:M40"/>
     <mergeCell ref="H39:J39"/>
     <mergeCell ref="K39:M39"/>
-    <mergeCell ref="F32:M32"/>
-    <mergeCell ref="F34:M34"/>
-    <mergeCell ref="F35:M35"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="K37:M37"/>
     <mergeCell ref="F25:M25"/>
     <mergeCell ref="F33:M33"/>
     <mergeCell ref="B2:M2"/>
@@ -4769,6 +5210,7 @@
     <mergeCell ref="F26:M26"/>
     <mergeCell ref="F27:M27"/>
     <mergeCell ref="F30:M30"/>
+    <mergeCell ref="F28:M28"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4783,8 +5225,8 @@
   </sheetPr>
   <dimension ref="B2:M15"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4794,255 +5236,255 @@
   <sheetData>
     <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="57" t="s">
-        <v>301</v>
-      </c>
-      <c r="C2" s="78" t="s">
-        <v>302</v>
-      </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
+        <v>299</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
     </row>
     <row r="3" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B3" s="58" t="s">
         <v>246</v>
       </c>
-      <c r="C3" s="76" t="s">
-        <v>316</v>
-      </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
+      <c r="C3" s="82" t="s">
+        <v>314</v>
+      </c>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="59" t="s">
-        <v>303</v>
-      </c>
-      <c r="C4" s="76" t="s">
-        <v>315</v>
-      </c>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
+        <v>301</v>
+      </c>
+      <c r="C4" s="82" t="s">
+        <v>313</v>
+      </c>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="59" t="s">
-        <v>304</v>
-      </c>
-      <c r="C5" s="76" t="s">
-        <v>317</v>
-      </c>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
+        <v>302</v>
+      </c>
+      <c r="C5" s="82" t="s">
+        <v>315</v>
+      </c>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="59" t="s">
-        <v>305</v>
-      </c>
-      <c r="C6" s="76" t="s">
-        <v>327</v>
-      </c>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="77"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
+        <v>303</v>
+      </c>
+      <c r="C6" s="82" t="s">
+        <v>325</v>
+      </c>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="83"/>
+      <c r="M6" s="83"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="59" t="s">
-        <v>306</v>
-      </c>
-      <c r="C7" s="76" t="s">
-        <v>326</v>
-      </c>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
+        <v>304</v>
+      </c>
+      <c r="C7" s="82" t="s">
+        <v>324</v>
+      </c>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="83"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>307</v>
-      </c>
-      <c r="C8" s="76" t="s">
-        <v>325</v>
-      </c>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="77"/>
+        <v>305</v>
+      </c>
+      <c r="C8" s="82" t="s">
+        <v>323</v>
+      </c>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="83"/>
+      <c r="M8" s="83"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>308</v>
-      </c>
-      <c r="C9" s="76" t="s">
-        <v>324</v>
-      </c>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="77"/>
-      <c r="K9" s="77"/>
-      <c r="L9" s="77"/>
-      <c r="M9" s="77"/>
+        <v>306</v>
+      </c>
+      <c r="C9" s="82" t="s">
+        <v>322</v>
+      </c>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="83"/>
+      <c r="L9" s="83"/>
+      <c r="M9" s="83"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>309</v>
-      </c>
-      <c r="C10" s="76" t="s">
-        <v>323</v>
-      </c>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="77"/>
-      <c r="K10" s="77"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="77"/>
+        <v>307</v>
+      </c>
+      <c r="C10" s="82" t="s">
+        <v>321</v>
+      </c>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="83"/>
+      <c r="K10" s="83"/>
+      <c r="L10" s="83"/>
+      <c r="M10" s="83"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>310</v>
-      </c>
-      <c r="C11" s="76" t="s">
-        <v>322</v>
-      </c>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="77"/>
-      <c r="L11" s="77"/>
-      <c r="M11" s="77"/>
+        <v>308</v>
+      </c>
+      <c r="C11" s="82" t="s">
+        <v>320</v>
+      </c>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="83"/>
+      <c r="L11" s="83"/>
+      <c r="M11" s="83"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>311</v>
-      </c>
-      <c r="C12" s="76" t="s">
-        <v>321</v>
-      </c>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77"/>
-      <c r="J12" s="77"/>
-      <c r="K12" s="77"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="77"/>
+        <v>309</v>
+      </c>
+      <c r="C12" s="82" t="s">
+        <v>319</v>
+      </c>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="83"/>
+      <c r="K12" s="83"/>
+      <c r="L12" s="83"/>
+      <c r="M12" s="83"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>312</v>
-      </c>
-      <c r="C13" s="76" t="s">
-        <v>320</v>
-      </c>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="77"/>
-      <c r="J13" s="77"/>
-      <c r="K13" s="77"/>
-      <c r="L13" s="77"/>
-      <c r="M13" s="77"/>
+        <v>310</v>
+      </c>
+      <c r="C13" s="82" t="s">
+        <v>318</v>
+      </c>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="83"/>
+      <c r="L13" s="83"/>
+      <c r="M13" s="83"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>313</v>
-      </c>
-      <c r="C14" s="76" t="s">
-        <v>319</v>
-      </c>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="77"/>
-      <c r="L14" s="77"/>
-      <c r="M14" s="77"/>
+        <v>311</v>
+      </c>
+      <c r="C14" s="82" t="s">
+        <v>317</v>
+      </c>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="83"/>
+      <c r="K14" s="83"/>
+      <c r="L14" s="83"/>
+      <c r="M14" s="83"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>314</v>
-      </c>
-      <c r="C15" s="76" t="s">
-        <v>318</v>
-      </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="77"/>
-      <c r="L15" s="77"/>
-      <c r="M15" s="77"/>
+        <v>312</v>
+      </c>
+      <c r="C15" s="82" t="s">
+        <v>316</v>
+      </c>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="83"/>
+      <c r="H15" s="83"/>
+      <c r="I15" s="83"/>
+      <c r="J15" s="83"/>
+      <c r="K15" s="83"/>
+      <c r="L15" s="83"/>
+      <c r="M15" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -5074,7 +5516,7 @@
   </sheetPr>
   <dimension ref="B1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="B14" sqref="B14:M19"/>
     </sheetView>
   </sheetViews>
@@ -5082,528 +5524,528 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="94" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+    </row>
+    <row r="3" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="97" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
+      <c r="M4" s="97"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
+      <c r="I5" s="97"/>
+      <c r="J5" s="97"/>
+      <c r="K5" s="97"/>
+      <c r="L5" s="97"/>
+      <c r="M5" s="97"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="98" t="s">
         <v>268</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-    </row>
-    <row r="3" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="91" t="s">
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="98"/>
+      <c r="H6" s="98"/>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="101" t="s">
         <v>269</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-      <c r="L5" s="91"/>
-      <c r="M5" s="91"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="92" t="s">
+      <c r="C7" s="101"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="101"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="101"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="101"/>
+      <c r="K8" s="101"/>
+      <c r="L8" s="101"/>
+      <c r="M8" s="101"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="101" t="s">
         <v>270</v>
       </c>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="95" t="s">
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="101"/>
+      <c r="K9" s="101"/>
+      <c r="L9" s="101"/>
+      <c r="M9" s="101"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="101" t="s">
         <v>271</v>
       </c>
-      <c r="C7" s="95"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="95"/>
-      <c r="M7" s="95"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="95"/>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
-      <c r="G8" s="95"/>
-      <c r="H8" s="95"/>
-      <c r="I8" s="95"/>
-      <c r="J8" s="95"/>
-      <c r="K8" s="95"/>
-      <c r="L8" s="95"/>
-      <c r="M8" s="95"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="95" t="s">
+      <c r="C10" s="101"/>
+      <c r="D10" s="101"/>
+      <c r="E10" s="101"/>
+      <c r="F10" s="101"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="101"/>
+      <c r="I10" s="101"/>
+      <c r="J10" s="101"/>
+      <c r="K10" s="101"/>
+      <c r="L10" s="101"/>
+      <c r="M10" s="101"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="101" t="s">
         <v>272</v>
       </c>
-      <c r="C9" s="95"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="95"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="95"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="95"/>
-      <c r="K9" s="95"/>
-      <c r="L9" s="95"/>
-      <c r="M9" s="95"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="95" t="s">
+      <c r="C11" s="101"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="101"/>
+      <c r="F11" s="101"/>
+      <c r="G11" s="101"/>
+      <c r="H11" s="101"/>
+      <c r="I11" s="101"/>
+      <c r="J11" s="101"/>
+      <c r="K11" s="101"/>
+      <c r="L11" s="101"/>
+      <c r="M11" s="101"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="101" t="s">
         <v>273</v>
       </c>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="95"/>
-      <c r="J10" s="95"/>
-      <c r="K10" s="95"/>
-      <c r="L10" s="95"/>
-      <c r="M10" s="95"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="95" t="s">
+      <c r="C12" s="101"/>
+      <c r="D12" s="101"/>
+      <c r="E12" s="101"/>
+      <c r="F12" s="101"/>
+      <c r="G12" s="101"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="101"/>
+      <c r="J12" s="101"/>
+      <c r="K12" s="101"/>
+      <c r="L12" s="101"/>
+      <c r="M12" s="101"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="102"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="102"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="102"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="97" t="s">
+        <v>291</v>
+      </c>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="97"/>
+      <c r="K14" s="97"/>
+      <c r="L14" s="97"/>
+      <c r="M14" s="97"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="97"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="97"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="97"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="97"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="97"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="97"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="97"/>
+      <c r="M16" s="97"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="97"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="97"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="97"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="97"/>
+      <c r="J17" s="97"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="97"/>
+      <c r="M17" s="97"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="97"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="97"/>
+      <c r="F18" s="97"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="97"/>
+      <c r="I18" s="97"/>
+      <c r="J18" s="97"/>
+      <c r="K18" s="97"/>
+      <c r="L18" s="97"/>
+      <c r="M18" s="97"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="97"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="97"/>
+      <c r="E19" s="97"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="97"/>
+      <c r="K19" s="97"/>
+      <c r="L19" s="97"/>
+      <c r="M19" s="97"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="97" t="s">
+        <v>289</v>
+      </c>
+      <c r="C20" s="97"/>
+      <c r="D20" s="97"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="97"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="97"/>
+      <c r="I20" s="97"/>
+      <c r="J20" s="97"/>
+      <c r="K20" s="97"/>
+      <c r="L20" s="97"/>
+      <c r="M20" s="97"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B21" s="97"/>
+      <c r="C21" s="97"/>
+      <c r="D21" s="97"/>
+      <c r="E21" s="97"/>
+      <c r="F21" s="97"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="97"/>
+      <c r="I21" s="97"/>
+      <c r="J21" s="97"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="97"/>
+      <c r="M21" s="97"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B22" s="97"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="97"/>
+      <c r="E22" s="97"/>
+      <c r="F22" s="97"/>
+      <c r="G22" s="97"/>
+      <c r="H22" s="97"/>
+      <c r="I22" s="97"/>
+      <c r="J22" s="97"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B23" s="97"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="G23" s="97"/>
+      <c r="H23" s="97"/>
+      <c r="I23" s="97"/>
+      <c r="J23" s="97"/>
+      <c r="K23" s="97"/>
+      <c r="L23" s="97"/>
+      <c r="M23" s="97"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B24" s="97"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="97"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="97"/>
+      <c r="I24" s="97"/>
+      <c r="J24" s="97"/>
+      <c r="K24" s="97"/>
+      <c r="L24" s="97"/>
+      <c r="M24" s="97"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B25" s="97"/>
+      <c r="C25" s="97"/>
+      <c r="D25" s="97"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="97"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="97"/>
+      <c r="I25" s="97"/>
+      <c r="J25" s="97"/>
+      <c r="K25" s="97"/>
+      <c r="L25" s="97"/>
+      <c r="M25" s="97"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B26" s="97" t="s">
         <v>274</v>
       </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="95"/>
-      <c r="K11" s="95"/>
-      <c r="L11" s="95"/>
-      <c r="M11" s="95"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="95" t="s">
+      <c r="C26" s="97"/>
+      <c r="D26" s="97"/>
+      <c r="E26" s="97"/>
+      <c r="F26" s="97"/>
+      <c r="G26" s="97"/>
+      <c r="H26" s="97"/>
+      <c r="I26" s="97"/>
+      <c r="J26" s="97"/>
+      <c r="K26" s="97"/>
+      <c r="L26" s="97"/>
+      <c r="M26" s="97"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B27" s="97"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="97"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="97"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="97"/>
+      <c r="K27" s="97"/>
+      <c r="L27" s="97"/>
+      <c r="M27" s="97"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B28" s="97"/>
+      <c r="C28" s="97"/>
+      <c r="D28" s="97"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="97"/>
+      <c r="G28" s="97"/>
+      <c r="H28" s="97"/>
+      <c r="I28" s="97"/>
+      <c r="J28" s="97"/>
+      <c r="K28" s="97"/>
+      <c r="L28" s="97"/>
+      <c r="M28" s="97"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B29" s="97"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="97"/>
+      <c r="E29" s="97"/>
+      <c r="F29" s="97"/>
+      <c r="G29" s="97"/>
+      <c r="H29" s="97"/>
+      <c r="I29" s="97"/>
+      <c r="J29" s="97"/>
+      <c r="K29" s="97"/>
+      <c r="L29" s="97"/>
+      <c r="M29" s="97"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B30" s="97" t="s">
         <v>275</v>
       </c>
-      <c r="C12" s="95"/>
-      <c r="D12" s="95"/>
-      <c r="E12" s="95"/>
-      <c r="F12" s="95"/>
-      <c r="G12" s="95"/>
-      <c r="H12" s="95"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="95"/>
-      <c r="K12" s="95"/>
-      <c r="L12" s="95"/>
-      <c r="M12" s="95"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="96"/>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="96"/>
-      <c r="G13" s="96"/>
-      <c r="H13" s="96"/>
-      <c r="I13" s="96"/>
-      <c r="J13" s="96"/>
-      <c r="K13" s="96"/>
-      <c r="L13" s="96"/>
-      <c r="M13" s="96"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="91" t="s">
-        <v>293</v>
-      </c>
-      <c r="C14" s="91"/>
-      <c r="D14" s="91"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="91"/>
-      <c r="G14" s="91"/>
-      <c r="H14" s="91"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="91"/>
-      <c r="K14" s="91"/>
-      <c r="L14" s="91"/>
-      <c r="M14" s="91"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="91"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="91"/>
-      <c r="I15" s="91"/>
-      <c r="J15" s="91"/>
-      <c r="K15" s="91"/>
-      <c r="L15" s="91"/>
-      <c r="M15" s="91"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="91"/>
-      <c r="C16" s="91"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="91"/>
-      <c r="K16" s="91"/>
-      <c r="L16" s="91"/>
-      <c r="M16" s="91"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="91"/>
-      <c r="C17" s="91"/>
-      <c r="D17" s="91"/>
-      <c r="E17" s="91"/>
-      <c r="F17" s="91"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="91"/>
-      <c r="I17" s="91"/>
-      <c r="J17" s="91"/>
-      <c r="K17" s="91"/>
-      <c r="L17" s="91"/>
-      <c r="M17" s="91"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="91"/>
-      <c r="C18" s="91"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="91"/>
-      <c r="F18" s="91"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="91"/>
-      <c r="I18" s="91"/>
-      <c r="J18" s="91"/>
-      <c r="K18" s="91"/>
-      <c r="L18" s="91"/>
-      <c r="M18" s="91"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="91"/>
-      <c r="E19" s="91"/>
-      <c r="F19" s="91"/>
-      <c r="G19" s="91"/>
-      <c r="H19" s="91"/>
-      <c r="I19" s="91"/>
-      <c r="J19" s="91"/>
-      <c r="K19" s="91"/>
-      <c r="L19" s="91"/>
-      <c r="M19" s="91"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="91" t="s">
-        <v>291</v>
-      </c>
-      <c r="C20" s="91"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="91"/>
-      <c r="G20" s="91"/>
-      <c r="H20" s="91"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="91"/>
-      <c r="K20" s="91"/>
-      <c r="L20" s="91"/>
-      <c r="M20" s="91"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="91"/>
-      <c r="C21" s="91"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="91"/>
-      <c r="G21" s="91"/>
-      <c r="H21" s="91"/>
-      <c r="I21" s="91"/>
-      <c r="J21" s="91"/>
-      <c r="K21" s="91"/>
-      <c r="L21" s="91"/>
-      <c r="M21" s="91"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="91"/>
-      <c r="C22" s="91"/>
-      <c r="D22" s="91"/>
-      <c r="E22" s="91"/>
-      <c r="F22" s="91"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="91"/>
-      <c r="I22" s="91"/>
-      <c r="J22" s="91"/>
-      <c r="K22" s="91"/>
-      <c r="L22" s="91"/>
-      <c r="M22" s="91"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="91"/>
-      <c r="C23" s="91"/>
-      <c r="D23" s="91"/>
-      <c r="E23" s="91"/>
-      <c r="F23" s="91"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="91"/>
-      <c r="I23" s="91"/>
-      <c r="J23" s="91"/>
-      <c r="K23" s="91"/>
-      <c r="L23" s="91"/>
-      <c r="M23" s="91"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="91"/>
-      <c r="C24" s="91"/>
-      <c r="D24" s="91"/>
-      <c r="E24" s="91"/>
-      <c r="F24" s="91"/>
-      <c r="G24" s="91"/>
-      <c r="H24" s="91"/>
-      <c r="I24" s="91"/>
-      <c r="J24" s="91"/>
-      <c r="K24" s="91"/>
-      <c r="L24" s="91"/>
-      <c r="M24" s="91"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="91"/>
-      <c r="C25" s="91"/>
-      <c r="D25" s="91"/>
-      <c r="E25" s="91"/>
-      <c r="F25" s="91"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="91"/>
-      <c r="I25" s="91"/>
-      <c r="J25" s="91"/>
-      <c r="K25" s="91"/>
-      <c r="L25" s="91"/>
-      <c r="M25" s="91"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="91" t="s">
+      <c r="C30" s="97"/>
+      <c r="D30" s="97"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="97"/>
+      <c r="G30" s="97"/>
+      <c r="H30" s="97"/>
+      <c r="I30" s="97"/>
+      <c r="J30" s="97"/>
+      <c r="K30" s="97"/>
+      <c r="L30" s="97"/>
+      <c r="M30" s="97"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B31" s="97"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="97"/>
+      <c r="E31" s="97"/>
+      <c r="F31" s="97"/>
+      <c r="G31" s="97"/>
+      <c r="H31" s="97"/>
+      <c r="I31" s="97"/>
+      <c r="J31" s="97"/>
+      <c r="K31" s="97"/>
+      <c r="L31" s="97"/>
+      <c r="M31" s="97"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B32" s="97"/>
+      <c r="C32" s="97"/>
+      <c r="D32" s="97"/>
+      <c r="E32" s="97"/>
+      <c r="F32" s="97"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="97"/>
+      <c r="J32" s="97"/>
+      <c r="K32" s="97"/>
+      <c r="L32" s="97"/>
+      <c r="M32" s="97"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B33" s="97"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="97"/>
+      <c r="E33" s="97"/>
+      <c r="F33" s="97"/>
+      <c r="G33" s="97"/>
+      <c r="H33" s="97"/>
+      <c r="I33" s="97"/>
+      <c r="J33" s="97"/>
+      <c r="K33" s="97"/>
+      <c r="L33" s="97"/>
+      <c r="M33" s="97"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B34" s="98" t="s">
         <v>276</v>
       </c>
-      <c r="C26" s="91"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="91"/>
-      <c r="F26" s="91"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="91"/>
-      <c r="I26" s="91"/>
-      <c r="J26" s="91"/>
-      <c r="K26" s="91"/>
-      <c r="L26" s="91"/>
-      <c r="M26" s="91"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="91"/>
-      <c r="C27" s="91"/>
-      <c r="D27" s="91"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="91"/>
-      <c r="G27" s="91"/>
-      <c r="H27" s="91"/>
-      <c r="I27" s="91"/>
-      <c r="J27" s="91"/>
-      <c r="K27" s="91"/>
-      <c r="L27" s="91"/>
-      <c r="M27" s="91"/>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="91"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="91"/>
-      <c r="E28" s="91"/>
-      <c r="F28" s="91"/>
-      <c r="G28" s="91"/>
-      <c r="H28" s="91"/>
-      <c r="I28" s="91"/>
-      <c r="J28" s="91"/>
-      <c r="K28" s="91"/>
-      <c r="L28" s="91"/>
-      <c r="M28" s="91"/>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="91"/>
-      <c r="C29" s="91"/>
-      <c r="D29" s="91"/>
-      <c r="E29" s="91"/>
-      <c r="F29" s="91"/>
-      <c r="G29" s="91"/>
-      <c r="H29" s="91"/>
-      <c r="I29" s="91"/>
-      <c r="J29" s="91"/>
-      <c r="K29" s="91"/>
-      <c r="L29" s="91"/>
-      <c r="M29" s="91"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="91" t="s">
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="83"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="83"/>
+      <c r="J34" s="83"/>
+      <c r="K34" s="83"/>
+      <c r="L34" s="83"/>
+      <c r="M34" s="83"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B35" s="99" t="s">
         <v>277</v>
       </c>
-      <c r="C30" s="91"/>
-      <c r="D30" s="91"/>
-      <c r="E30" s="91"/>
-      <c r="F30" s="91"/>
-      <c r="G30" s="91"/>
-      <c r="H30" s="91"/>
-      <c r="I30" s="91"/>
-      <c r="J30" s="91"/>
-      <c r="K30" s="91"/>
-      <c r="L30" s="91"/>
-      <c r="M30" s="91"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="91"/>
-      <c r="C31" s="91"/>
-      <c r="D31" s="91"/>
-      <c r="E31" s="91"/>
-      <c r="F31" s="91"/>
-      <c r="G31" s="91"/>
-      <c r="H31" s="91"/>
-      <c r="I31" s="91"/>
-      <c r="J31" s="91"/>
-      <c r="K31" s="91"/>
-      <c r="L31" s="91"/>
-      <c r="M31" s="91"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="91"/>
-      <c r="C32" s="91"/>
-      <c r="D32" s="91"/>
-      <c r="E32" s="91"/>
-      <c r="F32" s="91"/>
-      <c r="G32" s="91"/>
-      <c r="H32" s="91"/>
-      <c r="I32" s="91"/>
-      <c r="J32" s="91"/>
-      <c r="K32" s="91"/>
-      <c r="L32" s="91"/>
-      <c r="M32" s="91"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B33" s="91"/>
-      <c r="C33" s="91"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
-      <c r="G33" s="91"/>
-      <c r="H33" s="91"/>
-      <c r="I33" s="91"/>
-      <c r="J33" s="91"/>
-      <c r="K33" s="91"/>
-      <c r="L33" s="91"/>
-      <c r="M33" s="91"/>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B34" s="92" t="s">
+      <c r="C35" s="99"/>
+      <c r="D35" s="99"/>
+      <c r="E35" s="100">
+        <v>7</v>
+      </c>
+      <c r="F35" s="100"/>
+      <c r="G35" s="100"/>
+      <c r="H35" s="100"/>
+      <c r="I35" s="100"/>
+      <c r="J35" s="100"/>
+      <c r="K35" s="100"/>
+      <c r="L35" s="100"/>
+      <c r="M35" s="100"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B36" s="99" t="s">
         <v>278</v>
       </c>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="77"/>
-      <c r="L34" s="77"/>
-      <c r="M34" s="77"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B35" s="93" t="s">
-        <v>279</v>
-      </c>
-      <c r="C35" s="93"/>
-      <c r="D35" s="93"/>
-      <c r="E35" s="94">
-        <v>7</v>
-      </c>
-      <c r="F35" s="94"/>
-      <c r="G35" s="94"/>
-      <c r="H35" s="94"/>
-      <c r="I35" s="94"/>
-      <c r="J35" s="94"/>
-      <c r="K35" s="94"/>
-      <c r="L35" s="94"/>
-      <c r="M35" s="94"/>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B36" s="93" t="s">
-        <v>280</v>
-      </c>
-      <c r="C36" s="93"/>
-      <c r="D36" s="93"/>
-      <c r="E36" s="94">
+      <c r="C36" s="99"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="100">
         <v>8</v>
       </c>
-      <c r="F36" s="94"/>
-      <c r="G36" s="94"/>
-      <c r="H36" s="94"/>
-      <c r="I36" s="94"/>
-      <c r="J36" s="94"/>
-      <c r="K36" s="94"/>
-      <c r="L36" s="94"/>
-      <c r="M36" s="94"/>
+      <c r="F36" s="100"/>
+      <c r="G36" s="100"/>
+      <c r="H36" s="100"/>
+      <c r="I36" s="100"/>
+      <c r="J36" s="100"/>
+      <c r="K36" s="100"/>
+      <c r="L36" s="100"/>
+      <c r="M36" s="100"/>
     </row>
     <row r="37" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J37" s="51"/>
@@ -5612,26 +6054,26 @@
       <c r="M37" s="51"/>
     </row>
     <row r="38" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="88" t="s">
-        <v>281</v>
-      </c>
-      <c r="C38" s="88"/>
-      <c r="D38" s="88"/>
-      <c r="E38" s="88"/>
-      <c r="F38" s="88"/>
-      <c r="G38" s="88"/>
-      <c r="H38" s="88"/>
-      <c r="I38" s="88"/>
-      <c r="J38" s="89" t="s">
-        <v>292</v>
-      </c>
-      <c r="K38" s="88"/>
-      <c r="L38" s="88"/>
-      <c r="M38" s="88"/>
+      <c r="B38" s="94" t="s">
+        <v>279</v>
+      </c>
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
+      <c r="E38" s="94"/>
+      <c r="F38" s="94"/>
+      <c r="G38" s="94"/>
+      <c r="H38" s="94"/>
+      <c r="I38" s="94"/>
+      <c r="J38" s="95" t="s">
+        <v>290</v>
+      </c>
+      <c r="K38" s="94"/>
+      <c r="L38" s="94"/>
+      <c r="M38" s="94"/>
     </row>
     <row r="39" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B39" s="52" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C39" s="53" t="s">
         <v>163</v>
@@ -5654,72 +6096,72 @@
       <c r="I39" s="54" t="s">
         <v>169</v>
       </c>
-      <c r="J39" s="86" t="s">
-        <v>283</v>
-      </c>
-      <c r="K39" s="87"/>
-      <c r="L39" s="87"/>
-      <c r="M39" s="87"/>
+      <c r="J39" s="92" t="s">
+        <v>281</v>
+      </c>
+      <c r="K39" s="93"/>
+      <c r="L39" s="93"/>
+      <c r="M39" s="93"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
+        <v>282</v>
+      </c>
+      <c r="C40" s="86" t="s">
+        <v>283</v>
+      </c>
+      <c r="D40" s="87"/>
+      <c r="E40" s="87"/>
+      <c r="F40" s="87"/>
+      <c r="G40" s="87"/>
+      <c r="H40" s="87"/>
+      <c r="I40" s="88"/>
+      <c r="J40" s="96" t="s">
         <v>284</v>
       </c>
-      <c r="C40" s="80" t="s">
-        <v>285</v>
-      </c>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
-      <c r="G40" s="81"/>
-      <c r="H40" s="81"/>
-      <c r="I40" s="82"/>
-      <c r="J40" s="90" t="s">
-        <v>286</v>
-      </c>
-      <c r="K40" s="90"/>
-      <c r="L40" s="90"/>
-      <c r="M40" s="90"/>
+      <c r="K40" s="96"/>
+      <c r="L40" s="96"/>
+      <c r="M40" s="96"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" s="55">
         <v>0</v>
       </c>
-      <c r="C41" s="80" t="s">
-        <v>287</v>
-      </c>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="81"/>
-      <c r="G41" s="81"/>
-      <c r="H41" s="81"/>
-      <c r="I41" s="82"/>
-      <c r="J41" s="81" t="s">
-        <v>288</v>
-      </c>
-      <c r="K41" s="81"/>
-      <c r="L41" s="81"/>
-      <c r="M41" s="81"/>
+      <c r="C41" s="86" t="s">
+        <v>285</v>
+      </c>
+      <c r="D41" s="87"/>
+      <c r="E41" s="87"/>
+      <c r="F41" s="87"/>
+      <c r="G41" s="87"/>
+      <c r="H41" s="87"/>
+      <c r="I41" s="88"/>
+      <c r="J41" s="87" t="s">
+        <v>286</v>
+      </c>
+      <c r="K41" s="87"/>
+      <c r="L41" s="87"/>
+      <c r="M41" s="87"/>
     </row>
     <row r="42" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="56">
         <v>1</v>
       </c>
-      <c r="C42" s="83" t="s">
-        <v>289</v>
-      </c>
-      <c r="D42" s="84"/>
-      <c r="E42" s="84"/>
-      <c r="F42" s="84"/>
-      <c r="G42" s="84"/>
-      <c r="H42" s="84"/>
-      <c r="I42" s="84"/>
-      <c r="J42" s="85" t="s">
-        <v>290</v>
-      </c>
-      <c r="K42" s="84"/>
-      <c r="L42" s="84"/>
-      <c r="M42" s="84"/>
+      <c r="C42" s="89" t="s">
+        <v>287</v>
+      </c>
+      <c r="D42" s="90"/>
+      <c r="E42" s="90"/>
+      <c r="F42" s="90"/>
+      <c r="G42" s="90"/>
+      <c r="H42" s="90"/>
+      <c r="I42" s="90"/>
+      <c r="J42" s="91" t="s">
+        <v>288</v>
+      </c>
+      <c r="K42" s="90"/>
+      <c r="L42" s="90"/>
+      <c r="M42" s="90"/>
     </row>
     <row r="43" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -5755,4 +6197,345 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="78" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4438C717-898D-4D4B-9260-D99C6193E52E}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:M32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="85" t="s">
+        <v>329</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+    </row>
+    <row r="3" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L5" s="102" t="s">
+        <v>331</v>
+      </c>
+      <c r="M5" s="102"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="60"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="60"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="60"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="60"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="60"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="60"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="60"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D16" s="60" t="s">
+        <v>332</v>
+      </c>
+      <c r="E16" s="65"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="60" t="s">
+        <v>333</v>
+      </c>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D17" s="60"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="60"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60" t="s">
+        <v>334</v>
+      </c>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="60"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="L21" s="102" t="s">
+        <v>330</v>
+      </c>
+      <c r="M21" s="102"/>
+    </row>
+    <row r="24" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D24" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F25" s="116" t="s">
+        <v>338</v>
+      </c>
+      <c r="G25" s="117"/>
+      <c r="H25" s="117"/>
+      <c r="I25" s="117"/>
+      <c r="J25" s="117"/>
+      <c r="K25" s="118"/>
+    </row>
+    <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>337</v>
+      </c>
+      <c r="F26" s="116" t="s">
+        <v>339</v>
+      </c>
+      <c r="G26" s="117"/>
+      <c r="H26" s="118"/>
+      <c r="I26" s="119" t="s">
+        <v>340</v>
+      </c>
+      <c r="J26" s="119"/>
+      <c r="K26" s="120"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F27" s="108" t="s">
+        <v>341</v>
+      </c>
+      <c r="G27" s="109"/>
+      <c r="H27" s="110"/>
+      <c r="I27" s="103" t="s">
+        <v>342</v>
+      </c>
+      <c r="J27" s="103"/>
+      <c r="K27" s="104"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F28" s="111" t="s">
+        <v>343</v>
+      </c>
+      <c r="G28" s="101"/>
+      <c r="H28" s="112"/>
+      <c r="I28" s="83" t="s">
+        <v>344</v>
+      </c>
+      <c r="J28" s="83"/>
+      <c r="K28" s="105"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F29" s="111" t="s">
+        <v>345</v>
+      </c>
+      <c r="G29" s="101"/>
+      <c r="H29" s="112"/>
+      <c r="I29" s="83" t="s">
+        <v>347</v>
+      </c>
+      <c r="J29" s="83"/>
+      <c r="K29" s="105"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F30" s="111" t="s">
+        <v>348</v>
+      </c>
+      <c r="G30" s="101"/>
+      <c r="H30" s="112"/>
+      <c r="I30" s="83" t="s">
+        <v>346</v>
+      </c>
+      <c r="J30" s="83"/>
+      <c r="K30" s="105"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F31" s="111" t="s">
+        <v>349</v>
+      </c>
+      <c r="G31" s="101"/>
+      <c r="H31" s="112"/>
+      <c r="I31" s="83" t="s">
+        <v>350</v>
+      </c>
+      <c r="J31" s="83"/>
+      <c r="K31" s="105"/>
+    </row>
+    <row r="32" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F32" s="113" t="s">
+        <v>351</v>
+      </c>
+      <c r="G32" s="114"/>
+      <c r="H32" s="115"/>
+      <c r="I32" s="106" t="s">
+        <v>352</v>
+      </c>
+      <c r="J32" s="106"/>
+      <c r="K32" s="107"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="F25:K25"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="I31:K31"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
C06.00.10 - docs(src): Stepper motor use explained
Description of the TMC2660_DRIVER operation and the configuration
process
</commit_message>
<xml_diff>
--- a/hardware/boards/warehouse_v2/docs/Documentation_WH.xlsx
+++ b/hardware/boards/warehouse_v2/docs/Documentation_WH.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\Basurero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A96D80-0DCA-495D-BE11-589671D4C7C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1486ED4-24CF-4C79-90B3-A4A1E1F592E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{658C6C44-180A-4413-9118-4B5F379EEF28}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="3" activeTab="4" xr2:uid="{658C6C44-180A-4413-9118-4B5F379EEF28}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
     <sheet name="Registers" sheetId="2" r:id="rId2"/>
     <sheet name="Error List" sheetId="4" r:id="rId3"/>
     <sheet name="SPI Protocol" sheetId="3" r:id="rId4"/>
-    <sheet name="Map" sheetId="5" r:id="rId5"/>
+    <sheet name="Driving Stepper Motors" sheetId="6" r:id="rId5"/>
+    <sheet name="Map" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="362">
   <si>
     <t>Signal Name</t>
   </si>
@@ -1178,6 +1179,33 @@
   </si>
   <si>
     <t>Stepper1 -&gt; Dir1</t>
+  </si>
+  <si>
+    <t>Stepper Motor</t>
+  </si>
+  <si>
+    <t>The stepper motors are driven by the TMC2660. The TMC2660 is a driver for two-phase stepper motors with multiple industrial features. The driver includes high-resolution microstepping, sensorless mechanical load measurement, load measurement, load-adaptive power optimization, and low-resonance chopper operation. It si operated through either a standard SPI interface of a STEP/DIRECTION interface.</t>
+  </si>
+  <si>
+    <t>Configuration process:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The TMC2660 requires setting configuration parameters and mode bits through the SPI interface before the motor can be driven. The SPI interface also allows reading back status values and bits. </t>
+  </si>
+  <si>
+    <t>The warehouse_v2 hardware provides the TMC2660 with an initial configuration when the module is started. 5 SPI 24-bit transactions are performed to write the data to the 5 registers of the TMC2660. The default values for the initial configuration are located in the GOLDI_MODULE_CONFIG module in the TMC2660_rom structure. Once the hardware is started a FIFO structure loads the data into the SPI transmiter until the module has been programed.</t>
+  </si>
+  <si>
+    <t>After the initial configuration, the TMC2660 data can be modified by the user mid-operation using the three SPI registers in the TMC2660_DRIVER. Given that the TMC2600 returns the same data regardless of the rewritten register, three registers are enough to efficiently communicate with the chip. The SPI stream interface reacts to the write strobe of the lower register, meaning the SPI transmitter is loaded with the register's data when the SPI 0 data is modified.  A FIFO structure has been placed between the registers and SPI transmitter allowing the user to program up to 5 configuration word with the faster FPGA SPI interface without data losses.</t>
+  </si>
+  <si>
+    <t>Driving the stepper motor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To drive the stepper motor the STEP/DIRECTION interface of the TMC2660 is used. This interface is operated by the lower three registers in the TMC2660_DRIVER (the "motor speed" and "motor control") registers. </t>
+  </si>
+  <si>
+    <t>The motor speed registers contain the step signal frequency expressed in Hertz and the motor control register have two direction dependent enable signals. (If both are active the Dir1 takes precedent) Additionally, the stall bit reads the StallGuard2 information of the TMC2660 and flags a stall of the stepper motor. The power off bit temporarily disables the TMC2660 and allows the stepper motor to rotate freely  in case it has to be moved manualy.</t>
   </si>
 </sst>
 </file>
@@ -2091,7 +2119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2230,15 +2258,27 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2248,18 +2288,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2272,6 +2300,24 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2281,6 +2327,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2296,32 +2351,50 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2332,50 +2405,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4182,8 +4219,8 @@
   </sheetPr>
   <dimension ref="B2:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView topLeftCell="D9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4200,26 +4237,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="79" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="80" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="76"/>
+      <c r="C3" s="80"/>
       <c r="D3" s="1">
         <v>1</v>
       </c>
@@ -4234,10 +4271,10 @@
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="80" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="76"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="2" t="s">
         <v>155</v>
       </c>
@@ -4252,10 +4289,10 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="80" t="s">
         <v>154</v>
       </c>
-      <c r="C5" s="76"/>
+      <c r="C5" s="80"/>
       <c r="D5" s="3" t="s">
         <v>156</v>
       </c>
@@ -4270,34 +4307,34 @@
       <c r="M5" s="1"/>
     </row>
     <row r="7" spans="2:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="81" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
+      <c r="I7" s="81"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="77"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
     </row>
     <row r="9" spans="2:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="13"/>
@@ -4591,16 +4628,16 @@
       <c r="E19" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F19" s="74" t="s">
+      <c r="F19" s="72" t="s">
         <v>247</v>
       </c>
-      <c r="G19" s="74"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="74"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="74"/>
-      <c r="M19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="72"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="73"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="20" t="s">
@@ -4615,16 +4652,16 @@
       <c r="E20" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F20" s="74" t="s">
+      <c r="F20" s="72" t="s">
         <v>250</v>
       </c>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="72"/>
+      <c r="G20" s="72"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="72"/>
+      <c r="K20" s="72"/>
+      <c r="L20" s="72"/>
+      <c r="M20" s="73"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
@@ -4639,16 +4676,16 @@
       <c r="E21" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F21" s="74" t="s">
+      <c r="F21" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="74"/>
-      <c r="K21" s="74"/>
-      <c r="L21" s="74"/>
-      <c r="M21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="72"/>
+      <c r="K21" s="72"/>
+      <c r="L21" s="72"/>
+      <c r="M21" s="73"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
@@ -4663,16 +4700,16 @@
       <c r="E22" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F22" s="74" t="s">
+      <c r="F22" s="72" t="s">
         <v>249</v>
       </c>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="74"/>
-      <c r="L22" s="74"/>
-      <c r="M22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="72"/>
+      <c r="M22" s="73"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="20" t="s">
@@ -4717,16 +4754,16 @@
       <c r="E24" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F24" s="74" t="s">
+      <c r="F24" s="72" t="s">
         <v>251</v>
       </c>
-      <c r="G24" s="74"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="74"/>
-      <c r="K24" s="74"/>
-      <c r="L24" s="74"/>
-      <c r="M24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="72"/>
+      <c r="K24" s="72"/>
+      <c r="L24" s="72"/>
+      <c r="M24" s="73"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="20" t="s">
@@ -4741,16 +4778,16 @@
       <c r="E25" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F25" s="72" t="s">
+      <c r="F25" s="73" t="s">
         <v>292</v>
       </c>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="73"/>
-      <c r="M25" s="73"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="78"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="20" t="s">
@@ -4765,16 +4802,16 @@
       <c r="E26" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="F26" s="74" t="s">
+      <c r="F26" s="72" t="s">
         <v>252</v>
       </c>
-      <c r="G26" s="74"/>
-      <c r="H26" s="74"/>
-      <c r="I26" s="74"/>
-      <c r="J26" s="74"/>
-      <c r="K26" s="74"/>
-      <c r="L26" s="74"/>
-      <c r="M26" s="72"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="72"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="73"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="20" t="s">
@@ -4789,16 +4826,16 @@
       <c r="E27" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F27" s="74" t="s">
+      <c r="F27" s="72" t="s">
         <v>253</v>
       </c>
-      <c r="G27" s="74"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="74"/>
-      <c r="K27" s="74"/>
-      <c r="L27" s="74"/>
-      <c r="M27" s="72"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="72"/>
+      <c r="K27" s="72"/>
+      <c r="L27" s="72"/>
+      <c r="M27" s="73"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
@@ -4813,16 +4850,16 @@
       <c r="E28" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F28" s="72" t="s">
+      <c r="F28" s="73" t="s">
         <v>326</v>
       </c>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
-      <c r="J28" s="73"/>
-      <c r="K28" s="73"/>
-      <c r="L28" s="73"/>
-      <c r="M28" s="73"/>
+      <c r="G28" s="78"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="78"/>
+      <c r="J28" s="78"/>
+      <c r="K28" s="78"/>
+      <c r="L28" s="78"/>
+      <c r="M28" s="78"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="20" t="s">
@@ -4863,16 +4900,16 @@
       <c r="E30" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F30" s="74" t="s">
+      <c r="F30" s="72" t="s">
         <v>255</v>
       </c>
-      <c r="G30" s="74"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="74"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="74"/>
-      <c r="M30" s="72"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="72"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="72"/>
+      <c r="M30" s="73"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="20" t="s">
@@ -4917,16 +4954,16 @@
       <c r="E32" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F32" s="74" t="s">
+      <c r="F32" s="72" t="s">
         <v>251</v>
       </c>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="74"/>
-      <c r="K32" s="74"/>
-      <c r="L32" s="74"/>
-      <c r="M32" s="72"/>
+      <c r="G32" s="72"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="72"/>
+      <c r="K32" s="72"/>
+      <c r="L32" s="72"/>
+      <c r="M32" s="73"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="20" t="s">
@@ -4941,16 +4978,16 @@
       <c r="E33" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F33" s="74" t="s">
+      <c r="F33" s="72" t="s">
         <v>292</v>
       </c>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="72"/>
+      <c r="G33" s="72"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="72"/>
+      <c r="K33" s="72"/>
+      <c r="L33" s="72"/>
+      <c r="M33" s="73"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="20" t="s">
@@ -4965,16 +5002,16 @@
       <c r="E34" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="F34" s="74" t="s">
+      <c r="F34" s="72" t="s">
         <v>252</v>
       </c>
-      <c r="G34" s="74"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="74"/>
-      <c r="J34" s="74"/>
-      <c r="K34" s="74"/>
-      <c r="L34" s="74"/>
-      <c r="M34" s="72"/>
+      <c r="G34" s="72"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="72"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="73"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="20" t="s">
@@ -4989,16 +5026,16 @@
       <c r="E35" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="F35" s="74" t="s">
+      <c r="F35" s="72" t="s">
         <v>253</v>
       </c>
-      <c r="G35" s="74"/>
-      <c r="H35" s="74"/>
-      <c r="I35" s="74"/>
-      <c r="J35" s="74"/>
-      <c r="K35" s="74"/>
-      <c r="L35" s="74"/>
-      <c r="M35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="72"/>
+      <c r="L35" s="72"/>
+      <c r="M35" s="73"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="20" t="s">
@@ -5017,12 +5054,12 @@
       <c r="G36" s="23"/>
       <c r="H36" s="23"/>
       <c r="I36" s="23"/>
-      <c r="J36" s="74" t="s">
+      <c r="J36" s="72" t="s">
         <v>254</v>
       </c>
-      <c r="K36" s="74"/>
-      <c r="L36" s="74"/>
-      <c r="M36" s="72"/>
+      <c r="K36" s="72"/>
+      <c r="L36" s="72"/>
+      <c r="M36" s="73"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="20" t="s">
@@ -5043,16 +5080,16 @@
       <c r="G37" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="H37" s="80" t="s">
+      <c r="H37" s="74" t="s">
         <v>264</v>
       </c>
-      <c r="I37" s="80"/>
-      <c r="J37" s="80"/>
-      <c r="K37" s="80" t="s">
+      <c r="I37" s="74"/>
+      <c r="J37" s="74"/>
+      <c r="K37" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="L37" s="80"/>
-      <c r="M37" s="81"/>
+      <c r="L37" s="74"/>
+      <c r="M37" s="75"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="20" t="s">
@@ -5073,16 +5110,16 @@
       <c r="G38" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="H38" s="80" t="s">
+      <c r="H38" s="74" t="s">
         <v>264</v>
       </c>
-      <c r="I38" s="80"/>
-      <c r="J38" s="80"/>
-      <c r="K38" s="80" t="s">
+      <c r="I38" s="74"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="L38" s="80"/>
-      <c r="M38" s="81"/>
+      <c r="L38" s="74"/>
+      <c r="M38" s="75"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="20" t="s">
@@ -5103,16 +5140,16 @@
       <c r="G39" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="H39" s="80" t="s">
+      <c r="H39" s="74" t="s">
         <v>264</v>
       </c>
-      <c r="I39" s="80"/>
-      <c r="J39" s="80"/>
-      <c r="K39" s="80" t="s">
+      <c r="I39" s="74"/>
+      <c r="J39" s="74"/>
+      <c r="K39" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="L39" s="80"/>
-      <c r="M39" s="81"/>
+      <c r="L39" s="74"/>
+      <c r="M39" s="75"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="20" t="s">
@@ -5133,16 +5170,16 @@
       <c r="G40" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="H40" s="80" t="s">
+      <c r="H40" s="74" t="s">
         <v>264</v>
       </c>
-      <c r="I40" s="80"/>
-      <c r="J40" s="80"/>
-      <c r="K40" s="80" t="s">
+      <c r="I40" s="74"/>
+      <c r="J40" s="74"/>
+      <c r="K40" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="L40" s="80"/>
-      <c r="M40" s="81"/>
+      <c r="L40" s="74"/>
+      <c r="M40" s="75"/>
     </row>
     <row r="41" spans="2:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="25" t="s">
@@ -5163,16 +5200,16 @@
       <c r="G41" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="H41" s="78" t="s">
+      <c r="H41" s="76" t="s">
         <v>264</v>
       </c>
-      <c r="I41" s="78"/>
-      <c r="J41" s="78"/>
-      <c r="K41" s="78" t="s">
+      <c r="I41" s="76"/>
+      <c r="J41" s="76"/>
+      <c r="K41" s="76" t="s">
         <v>265</v>
       </c>
-      <c r="L41" s="78"/>
-      <c r="M41" s="79"/>
+      <c r="L41" s="76"/>
+      <c r="M41" s="77"/>
     </row>
     <row r="42" spans="2:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C42" s="29"/>
@@ -5181,20 +5218,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="F32:M32"/>
-    <mergeCell ref="F34:M34"/>
-    <mergeCell ref="F35:M35"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="K39:M39"/>
     <mergeCell ref="F25:M25"/>
     <mergeCell ref="F33:M33"/>
     <mergeCell ref="B2:M2"/>
@@ -5211,6 +5234,20 @@
     <mergeCell ref="F27:M27"/>
     <mergeCell ref="F30:M30"/>
     <mergeCell ref="F28:M28"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="F32:M32"/>
+    <mergeCell ref="F34:M34"/>
+    <mergeCell ref="F35:M35"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="K37:M37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5516,487 +5553,487 @@
   </sheetPr>
   <dimension ref="B1:M43"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:M19"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="87" t="s">
         <v>266</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
     </row>
     <row r="3" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="86" t="s">
         <v>267</v>
       </c>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="86"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="97"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
-      <c r="M4" s="97"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="97"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="88" t="s">
         <v>268</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="88"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="89" t="s">
         <v>269</v>
       </c>
-      <c r="C7" s="101"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="101"/>
-      <c r="M7" s="101"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+      <c r="L7" s="89"/>
+      <c r="M7" s="89"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="101"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
-      <c r="M8" s="101"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="89"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="89"/>
+      <c r="L8" s="89"/>
+      <c r="M8" s="89"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="89" t="s">
         <v>270</v>
       </c>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
-      <c r="M9" s="101"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="89"/>
+      <c r="M9" s="89"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="101" t="s">
+      <c r="B10" s="89" t="s">
         <v>271</v>
       </c>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101"/>
-      <c r="M10" s="101"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="89"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="89" t="s">
         <v>272</v>
       </c>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="101"/>
-      <c r="I11" s="101"/>
-      <c r="J11" s="101"/>
-      <c r="K11" s="101"/>
-      <c r="L11" s="101"/>
-      <c r="M11" s="101"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="89"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="89"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="101" t="s">
+      <c r="B12" s="89" t="s">
         <v>273</v>
       </c>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="101"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="101"/>
-      <c r="K12" s="101"/>
-      <c r="L12" s="101"/>
-      <c r="M12" s="101"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="102"/>
-      <c r="C13" s="102"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="102"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="102"/>
-      <c r="L13" s="102"/>
-      <c r="M13" s="102"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="90"/>
+      <c r="M13" s="90"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="86" t="s">
         <v>291</v>
       </c>
-      <c r="C14" s="97"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="97"/>
-      <c r="G14" s="97"/>
-      <c r="H14" s="97"/>
-      <c r="I14" s="97"/>
-      <c r="J14" s="97"/>
-      <c r="K14" s="97"/>
-      <c r="L14" s="97"/>
-      <c r="M14" s="97"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="86"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="97"/>
-      <c r="C15" s="97"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="97"/>
-      <c r="G15" s="97"/>
-      <c r="H15" s="97"/>
-      <c r="I15" s="97"/>
-      <c r="J15" s="97"/>
-      <c r="K15" s="97"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="97"/>
+      <c r="B15" s="86"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="86"/>
+      <c r="M15" s="86"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="97"/>
-      <c r="C16" s="97"/>
-      <c r="D16" s="97"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="97"/>
-      <c r="G16" s="97"/>
-      <c r="H16" s="97"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="97"/>
-      <c r="K16" s="97"/>
-      <c r="L16" s="97"/>
-      <c r="M16" s="97"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="86"/>
+      <c r="M16" s="86"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="97"/>
-      <c r="C17" s="97"/>
-      <c r="D17" s="97"/>
-      <c r="E17" s="97"/>
-      <c r="F17" s="97"/>
-      <c r="G17" s="97"/>
-      <c r="H17" s="97"/>
-      <c r="I17" s="97"/>
-      <c r="J17" s="97"/>
-      <c r="K17" s="97"/>
-      <c r="L17" s="97"/>
-      <c r="M17" s="97"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="86"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="97"/>
-      <c r="C18" s="97"/>
-      <c r="D18" s="97"/>
-      <c r="E18" s="97"/>
-      <c r="F18" s="97"/>
-      <c r="G18" s="97"/>
-      <c r="H18" s="97"/>
-      <c r="I18" s="97"/>
-      <c r="J18" s="97"/>
-      <c r="K18" s="97"/>
-      <c r="L18" s="97"/>
-      <c r="M18" s="97"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="86"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B19" s="97"/>
-      <c r="C19" s="97"/>
-      <c r="D19" s="97"/>
-      <c r="E19" s="97"/>
-      <c r="F19" s="97"/>
-      <c r="G19" s="97"/>
-      <c r="H19" s="97"/>
-      <c r="I19" s="97"/>
-      <c r="J19" s="97"/>
-      <c r="K19" s="97"/>
-      <c r="L19" s="97"/>
-      <c r="M19" s="97"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="86"/>
+      <c r="H19" s="86"/>
+      <c r="I19" s="86"/>
+      <c r="J19" s="86"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="86"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="86" t="s">
         <v>289</v>
       </c>
-      <c r="C20" s="97"/>
-      <c r="D20" s="97"/>
-      <c r="E20" s="97"/>
-      <c r="F20" s="97"/>
-      <c r="G20" s="97"/>
-      <c r="H20" s="97"/>
-      <c r="I20" s="97"/>
-      <c r="J20" s="97"/>
-      <c r="K20" s="97"/>
-      <c r="L20" s="97"/>
-      <c r="M20" s="97"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="86"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="86"/>
+      <c r="K20" s="86"/>
+      <c r="L20" s="86"/>
+      <c r="M20" s="86"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="97"/>
-      <c r="C21" s="97"/>
-      <c r="D21" s="97"/>
-      <c r="E21" s="97"/>
-      <c r="F21" s="97"/>
-      <c r="G21" s="97"/>
-      <c r="H21" s="97"/>
-      <c r="I21" s="97"/>
-      <c r="J21" s="97"/>
-      <c r="K21" s="97"/>
-      <c r="L21" s="97"/>
-      <c r="M21" s="97"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="86"/>
+      <c r="I21" s="86"/>
+      <c r="J21" s="86"/>
+      <c r="K21" s="86"/>
+      <c r="L21" s="86"/>
+      <c r="M21" s="86"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="97"/>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="97"/>
-      <c r="G22" s="97"/>
-      <c r="H22" s="97"/>
-      <c r="I22" s="97"/>
-      <c r="J22" s="97"/>
-      <c r="K22" s="97"/>
-      <c r="L22" s="97"/>
-      <c r="M22" s="97"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="86"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="86"/>
+      <c r="K22" s="86"/>
+      <c r="L22" s="86"/>
+      <c r="M22" s="86"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="97"/>
-      <c r="C23" s="97"/>
-      <c r="D23" s="97"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="97"/>
-      <c r="G23" s="97"/>
-      <c r="H23" s="97"/>
-      <c r="I23" s="97"/>
-      <c r="J23" s="97"/>
-      <c r="K23" s="97"/>
-      <c r="L23" s="97"/>
-      <c r="M23" s="97"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="86"/>
+      <c r="J23" s="86"/>
+      <c r="K23" s="86"/>
+      <c r="L23" s="86"/>
+      <c r="M23" s="86"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="97"/>
-      <c r="C24" s="97"/>
-      <c r="D24" s="97"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="97"/>
-      <c r="G24" s="97"/>
-      <c r="H24" s="97"/>
-      <c r="I24" s="97"/>
-      <c r="J24" s="97"/>
-      <c r="K24" s="97"/>
-      <c r="L24" s="97"/>
-      <c r="M24" s="97"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="86"/>
+      <c r="K24" s="86"/>
+      <c r="L24" s="86"/>
+      <c r="M24" s="86"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="97"/>
-      <c r="C25" s="97"/>
-      <c r="D25" s="97"/>
-      <c r="E25" s="97"/>
-      <c r="F25" s="97"/>
-      <c r="G25" s="97"/>
-      <c r="H25" s="97"/>
-      <c r="I25" s="97"/>
-      <c r="J25" s="97"/>
-      <c r="K25" s="97"/>
-      <c r="L25" s="97"/>
-      <c r="M25" s="97"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
+      <c r="H25" s="86"/>
+      <c r="I25" s="86"/>
+      <c r="J25" s="86"/>
+      <c r="K25" s="86"/>
+      <c r="L25" s="86"/>
+      <c r="M25" s="86"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="97" t="s">
+      <c r="B26" s="86" t="s">
         <v>274</v>
       </c>
-      <c r="C26" s="97"/>
-      <c r="D26" s="97"/>
-      <c r="E26" s="97"/>
-      <c r="F26" s="97"/>
-      <c r="G26" s="97"/>
-      <c r="H26" s="97"/>
-      <c r="I26" s="97"/>
-      <c r="J26" s="97"/>
-      <c r="K26" s="97"/>
-      <c r="L26" s="97"/>
-      <c r="M26" s="97"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="86"/>
+      <c r="I26" s="86"/>
+      <c r="J26" s="86"/>
+      <c r="K26" s="86"/>
+      <c r="L26" s="86"/>
+      <c r="M26" s="86"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="97"/>
-      <c r="C27" s="97"/>
-      <c r="D27" s="97"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="97"/>
-      <c r="G27" s="97"/>
-      <c r="H27" s="97"/>
-      <c r="I27" s="97"/>
-      <c r="J27" s="97"/>
-      <c r="K27" s="97"/>
-      <c r="L27" s="97"/>
-      <c r="M27" s="97"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="86"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
+      <c r="H27" s="86"/>
+      <c r="I27" s="86"/>
+      <c r="J27" s="86"/>
+      <c r="K27" s="86"/>
+      <c r="L27" s="86"/>
+      <c r="M27" s="86"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="97"/>
-      <c r="C28" s="97"/>
-      <c r="D28" s="97"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="97"/>
-      <c r="G28" s="97"/>
-      <c r="H28" s="97"/>
-      <c r="I28" s="97"/>
-      <c r="J28" s="97"/>
-      <c r="K28" s="97"/>
-      <c r="L28" s="97"/>
-      <c r="M28" s="97"/>
+      <c r="B28" s="86"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="86"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="97"/>
-      <c r="C29" s="97"/>
-      <c r="D29" s="97"/>
-      <c r="E29" s="97"/>
-      <c r="F29" s="97"/>
-      <c r="G29" s="97"/>
-      <c r="H29" s="97"/>
-      <c r="I29" s="97"/>
-      <c r="J29" s="97"/>
-      <c r="K29" s="97"/>
-      <c r="L29" s="97"/>
-      <c r="M29" s="97"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="86"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
+      <c r="H29" s="86"/>
+      <c r="I29" s="86"/>
+      <c r="J29" s="86"/>
+      <c r="K29" s="86"/>
+      <c r="L29" s="86"/>
+      <c r="M29" s="86"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="97" t="s">
+      <c r="B30" s="86" t="s">
         <v>275</v>
       </c>
-      <c r="C30" s="97"/>
-      <c r="D30" s="97"/>
-      <c r="E30" s="97"/>
-      <c r="F30" s="97"/>
-      <c r="G30" s="97"/>
-      <c r="H30" s="97"/>
-      <c r="I30" s="97"/>
-      <c r="J30" s="97"/>
-      <c r="K30" s="97"/>
-      <c r="L30" s="97"/>
-      <c r="M30" s="97"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="86"/>
+      <c r="G30" s="86"/>
+      <c r="H30" s="86"/>
+      <c r="I30" s="86"/>
+      <c r="J30" s="86"/>
+      <c r="K30" s="86"/>
+      <c r="L30" s="86"/>
+      <c r="M30" s="86"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="97"/>
-      <c r="C31" s="97"/>
-      <c r="D31" s="97"/>
-      <c r="E31" s="97"/>
-      <c r="F31" s="97"/>
-      <c r="G31" s="97"/>
-      <c r="H31" s="97"/>
-      <c r="I31" s="97"/>
-      <c r="J31" s="97"/>
-      <c r="K31" s="97"/>
-      <c r="L31" s="97"/>
-      <c r="M31" s="97"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="86"/>
+      <c r="I31" s="86"/>
+      <c r="J31" s="86"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="86"/>
+      <c r="M31" s="86"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="97"/>
-      <c r="C32" s="97"/>
-      <c r="D32" s="97"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="97"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="97"/>
-      <c r="I32" s="97"/>
-      <c r="J32" s="97"/>
-      <c r="K32" s="97"/>
-      <c r="L32" s="97"/>
-      <c r="M32" s="97"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="86"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="86"/>
+      <c r="H32" s="86"/>
+      <c r="I32" s="86"/>
+      <c r="J32" s="86"/>
+      <c r="K32" s="86"/>
+      <c r="L32" s="86"/>
+      <c r="M32" s="86"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B33" s="97"/>
-      <c r="C33" s="97"/>
-      <c r="D33" s="97"/>
-      <c r="E33" s="97"/>
-      <c r="F33" s="97"/>
-      <c r="G33" s="97"/>
-      <c r="H33" s="97"/>
-      <c r="I33" s="97"/>
-      <c r="J33" s="97"/>
-      <c r="K33" s="97"/>
-      <c r="L33" s="97"/>
-      <c r="M33" s="97"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="86"/>
+      <c r="E33" s="86"/>
+      <c r="F33" s="86"/>
+      <c r="G33" s="86"/>
+      <c r="H33" s="86"/>
+      <c r="I33" s="86"/>
+      <c r="J33" s="86"/>
+      <c r="K33" s="86"/>
+      <c r="L33" s="86"/>
+      <c r="M33" s="86"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B34" s="98" t="s">
+      <c r="B34" s="88" t="s">
         <v>276</v>
       </c>
       <c r="C34" s="83"/>
@@ -6012,40 +6049,40 @@
       <c r="M34" s="83"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B35" s="99" t="s">
+      <c r="B35" s="96" t="s">
         <v>277</v>
       </c>
-      <c r="C35" s="99"/>
-      <c r="D35" s="99"/>
-      <c r="E35" s="100">
+      <c r="C35" s="96"/>
+      <c r="D35" s="96"/>
+      <c r="E35" s="97">
         <v>7</v>
       </c>
-      <c r="F35" s="100"/>
-      <c r="G35" s="100"/>
-      <c r="H35" s="100"/>
-      <c r="I35" s="100"/>
-      <c r="J35" s="100"/>
-      <c r="K35" s="100"/>
-      <c r="L35" s="100"/>
-      <c r="M35" s="100"/>
+      <c r="F35" s="97"/>
+      <c r="G35" s="97"/>
+      <c r="H35" s="97"/>
+      <c r="I35" s="97"/>
+      <c r="J35" s="97"/>
+      <c r="K35" s="97"/>
+      <c r="L35" s="97"/>
+      <c r="M35" s="97"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B36" s="99" t="s">
+      <c r="B36" s="96" t="s">
         <v>278</v>
       </c>
-      <c r="C36" s="99"/>
-      <c r="D36" s="99"/>
-      <c r="E36" s="100">
+      <c r="C36" s="96"/>
+      <c r="D36" s="96"/>
+      <c r="E36" s="97">
         <v>8</v>
       </c>
-      <c r="F36" s="100"/>
-      <c r="G36" s="100"/>
-      <c r="H36" s="100"/>
-      <c r="I36" s="100"/>
-      <c r="J36" s="100"/>
-      <c r="K36" s="100"/>
-      <c r="L36" s="100"/>
-      <c r="M36" s="100"/>
+      <c r="F36" s="97"/>
+      <c r="G36" s="97"/>
+      <c r="H36" s="97"/>
+      <c r="I36" s="97"/>
+      <c r="J36" s="97"/>
+      <c r="K36" s="97"/>
+      <c r="L36" s="97"/>
+      <c r="M36" s="97"/>
     </row>
     <row r="37" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J37" s="51"/>
@@ -6054,22 +6091,22 @@
       <c r="M37" s="51"/>
     </row>
     <row r="38" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="94" t="s">
+      <c r="B38" s="87" t="s">
         <v>279</v>
       </c>
-      <c r="C38" s="94"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="94"/>
-      <c r="F38" s="94"/>
-      <c r="G38" s="94"/>
-      <c r="H38" s="94"/>
-      <c r="I38" s="94"/>
-      <c r="J38" s="95" t="s">
+      <c r="C38" s="87"/>
+      <c r="D38" s="87"/>
+      <c r="E38" s="87"/>
+      <c r="F38" s="87"/>
+      <c r="G38" s="87"/>
+      <c r="H38" s="87"/>
+      <c r="I38" s="87"/>
+      <c r="J38" s="91" t="s">
         <v>290</v>
       </c>
-      <c r="K38" s="94"/>
-      <c r="L38" s="94"/>
-      <c r="M38" s="94"/>
+      <c r="K38" s="87"/>
+      <c r="L38" s="87"/>
+      <c r="M38" s="87"/>
     </row>
     <row r="39" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B39" s="52" t="s">
@@ -6096,76 +6133,91 @@
       <c r="I39" s="54" t="s">
         <v>169</v>
       </c>
-      <c r="J39" s="92" t="s">
+      <c r="J39" s="101" t="s">
         <v>281</v>
       </c>
-      <c r="K39" s="93"/>
-      <c r="L39" s="93"/>
-      <c r="M39" s="93"/>
+      <c r="K39" s="102"/>
+      <c r="L39" s="102"/>
+      <c r="M39" s="102"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>282</v>
       </c>
-      <c r="C40" s="86" t="s">
+      <c r="C40" s="92" t="s">
         <v>283</v>
       </c>
-      <c r="D40" s="87"/>
-      <c r="E40" s="87"/>
-      <c r="F40" s="87"/>
-      <c r="G40" s="87"/>
-      <c r="H40" s="87"/>
-      <c r="I40" s="88"/>
-      <c r="J40" s="96" t="s">
+      <c r="D40" s="93"/>
+      <c r="E40" s="93"/>
+      <c r="F40" s="93"/>
+      <c r="G40" s="93"/>
+      <c r="H40" s="93"/>
+      <c r="I40" s="94"/>
+      <c r="J40" s="95" t="s">
         <v>284</v>
       </c>
-      <c r="K40" s="96"/>
-      <c r="L40" s="96"/>
-      <c r="M40" s="96"/>
+      <c r="K40" s="95"/>
+      <c r="L40" s="95"/>
+      <c r="M40" s="95"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B41" s="55">
         <v>0</v>
       </c>
-      <c r="C41" s="86" t="s">
+      <c r="C41" s="92" t="s">
         <v>285</v>
       </c>
-      <c r="D41" s="87"/>
-      <c r="E41" s="87"/>
-      <c r="F41" s="87"/>
-      <c r="G41" s="87"/>
-      <c r="H41" s="87"/>
-      <c r="I41" s="88"/>
-      <c r="J41" s="87" t="s">
+      <c r="D41" s="93"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="93"/>
+      <c r="G41" s="93"/>
+      <c r="H41" s="93"/>
+      <c r="I41" s="94"/>
+      <c r="J41" s="93" t="s">
         <v>286</v>
       </c>
-      <c r="K41" s="87"/>
-      <c r="L41" s="87"/>
-      <c r="M41" s="87"/>
+      <c r="K41" s="93"/>
+      <c r="L41" s="93"/>
+      <c r="M41" s="93"/>
     </row>
     <row r="42" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="56">
         <v>1</v>
       </c>
-      <c r="C42" s="89" t="s">
+      <c r="C42" s="98" t="s">
         <v>287</v>
       </c>
-      <c r="D42" s="90"/>
-      <c r="E42" s="90"/>
-      <c r="F42" s="90"/>
-      <c r="G42" s="90"/>
-      <c r="H42" s="90"/>
-      <c r="I42" s="90"/>
-      <c r="J42" s="91" t="s">
+      <c r="D42" s="99"/>
+      <c r="E42" s="99"/>
+      <c r="F42" s="99"/>
+      <c r="G42" s="99"/>
+      <c r="H42" s="99"/>
+      <c r="I42" s="99"/>
+      <c r="J42" s="100" t="s">
         <v>288</v>
       </c>
-      <c r="K42" s="90"/>
-      <c r="L42" s="90"/>
-      <c r="M42" s="90"/>
+      <c r="K42" s="99"/>
+      <c r="L42" s="99"/>
+      <c r="M42" s="99"/>
     </row>
     <row r="43" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="C42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="C40:I40"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="B30:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:M35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:M36"/>
     <mergeCell ref="B26:M29"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M5"/>
@@ -6178,21 +6230,6 @@
     <mergeCell ref="B13:M13"/>
     <mergeCell ref="B14:M19"/>
     <mergeCell ref="B20:M25"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="C40:I40"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="B30:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:M35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:M36"/>
-    <mergeCell ref="C41:I41"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="C42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="J39:M39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="78" orientation="portrait" r:id="rId1"/>
@@ -6200,13 +6237,508 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CDE4519-60A4-44BA-AF7F-1853D42F5297}">
+  <dimension ref="B1:M33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="87" t="s">
+        <v>353</v>
+      </c>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+    </row>
+    <row r="3" spans="2:13" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="122" t="s">
+        <v>354</v>
+      </c>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="123"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="123"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="123"/>
+      <c r="L5" s="123"/>
+      <c r="M5" s="123"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="123"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="123"/>
+      <c r="J6" s="123"/>
+      <c r="K6" s="123"/>
+      <c r="L6" s="123"/>
+      <c r="M6" s="123"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="123"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="123"/>
+      <c r="E7" s="123"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="123"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="123"/>
+      <c r="L7" s="123"/>
+      <c r="M7" s="123"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="88" t="s">
+        <v>355</v>
+      </c>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="88"/>
+      <c r="M8" s="88"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="86" t="s">
+        <v>356</v>
+      </c>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="86"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="86"/>
+      <c r="M10" s="86"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="121"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="121"/>
+      <c r="I11" s="121"/>
+      <c r="J11" s="121"/>
+      <c r="K11" s="121"/>
+      <c r="L11" s="121"/>
+      <c r="M11" s="121"/>
+    </row>
+    <row r="12" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="86" t="s">
+        <v>357</v>
+      </c>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="86"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="86"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="86"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="86"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="86"/>
+      <c r="M15" s="86"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="86"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="86"/>
+      <c r="M16" s="86"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="86" t="s">
+        <v>358</v>
+      </c>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="86"/>
+    </row>
+    <row r="18" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="86"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="86"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="86"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="86"/>
+      <c r="H19" s="86"/>
+      <c r="I19" s="86"/>
+      <c r="J19" s="86"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="86"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="86"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="86"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="86"/>
+      <c r="K20" s="86"/>
+      <c r="L20" s="86"/>
+      <c r="M20" s="86"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B21" s="86"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="86"/>
+      <c r="I21" s="86"/>
+      <c r="J21" s="86"/>
+      <c r="K21" s="86"/>
+      <c r="L21" s="86"/>
+      <c r="M21" s="86"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B22" s="86"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="86"/>
+      <c r="I22" s="86"/>
+      <c r="J22" s="86"/>
+      <c r="K22" s="86"/>
+      <c r="L22" s="86"/>
+      <c r="M22" s="86"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B23" s="86"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="86"/>
+      <c r="J23" s="86"/>
+      <c r="K23" s="86"/>
+      <c r="L23" s="86"/>
+      <c r="M23" s="86"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B24" s="88" t="s">
+        <v>359</v>
+      </c>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B25" s="86" t="s">
+        <v>360</v>
+      </c>
+      <c r="C25" s="86"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
+      <c r="H25" s="86"/>
+      <c r="I25" s="86"/>
+      <c r="J25" s="86"/>
+      <c r="K25" s="86"/>
+      <c r="L25" s="86"/>
+      <c r="M25" s="86"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B26" s="86"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="86"/>
+      <c r="I26" s="86"/>
+      <c r="J26" s="86"/>
+      <c r="K26" s="86"/>
+      <c r="L26" s="86"/>
+      <c r="M26" s="86"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B27" s="86"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="86"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
+      <c r="H27" s="86"/>
+      <c r="I27" s="86"/>
+      <c r="J27" s="86"/>
+      <c r="K27" s="86"/>
+      <c r="L27" s="86"/>
+      <c r="M27" s="86"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B28" s="86" t="s">
+        <v>361</v>
+      </c>
+      <c r="C28" s="86"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="86"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B29" s="86"/>
+      <c r="C29" s="86"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
+      <c r="H29" s="86"/>
+      <c r="I29" s="86"/>
+      <c r="J29" s="86"/>
+      <c r="K29" s="86"/>
+      <c r="L29" s="86"/>
+      <c r="M29" s="86"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B30" s="86"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="86"/>
+      <c r="G30" s="86"/>
+      <c r="H30" s="86"/>
+      <c r="I30" s="86"/>
+      <c r="J30" s="86"/>
+      <c r="K30" s="86"/>
+      <c r="L30" s="86"/>
+      <c r="M30" s="86"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B31" s="86"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="86"/>
+      <c r="I31" s="86"/>
+      <c r="J31" s="86"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="86"/>
+      <c r="M31" s="86"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B32" s="86"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="86"/>
+      <c r="E32" s="86"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="86"/>
+      <c r="H32" s="86"/>
+      <c r="I32" s="86"/>
+      <c r="J32" s="86"/>
+      <c r="K32" s="86"/>
+      <c r="L32" s="86"/>
+      <c r="M32" s="86"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B33" s="86"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="86"/>
+      <c r="E33" s="86"/>
+      <c r="F33" s="86"/>
+      <c r="G33" s="86"/>
+      <c r="H33" s="86"/>
+      <c r="I33" s="86"/>
+      <c r="J33" s="86"/>
+      <c r="K33" s="86"/>
+      <c r="L33" s="86"/>
+      <c r="M33" s="86"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B24:M24"/>
+    <mergeCell ref="B25:M27"/>
+    <mergeCell ref="B28:M33"/>
+    <mergeCell ref="B12:M16"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="B17:M23"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M7"/>
+    <mergeCell ref="B8:M8"/>
+    <mergeCell ref="B9:M10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4438C717-898D-4D4B-9260-D99C6193E52E}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
@@ -6233,10 +6765,10 @@
     </row>
     <row r="3" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="L5" s="102" t="s">
+      <c r="L5" s="90" t="s">
         <v>331</v>
       </c>
-      <c r="M5" s="102"/>
+      <c r="M5" s="90"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="D7" s="60"/>
@@ -6406,10 +6938,10 @@
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="L21" s="102" t="s">
+      <c r="L21" s="90" t="s">
         <v>330</v>
       </c>
-      <c r="M21" s="102"/>
+      <c r="M21" s="90"/>
     </row>
     <row r="24" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D24" t="s">
@@ -6417,110 +6949,104 @@
       </c>
     </row>
     <row r="25" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F25" s="116" t="s">
+      <c r="F25" s="103" t="s">
         <v>338</v>
       </c>
-      <c r="G25" s="117"/>
-      <c r="H25" s="117"/>
-      <c r="I25" s="117"/>
-      <c r="J25" s="117"/>
-      <c r="K25" s="118"/>
+      <c r="G25" s="104"/>
+      <c r="H25" s="104"/>
+      <c r="I25" s="104"/>
+      <c r="J25" s="104"/>
+      <c r="K25" s="105"/>
     </row>
     <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>337</v>
       </c>
-      <c r="F26" s="116" t="s">
+      <c r="F26" s="103" t="s">
         <v>339</v>
       </c>
-      <c r="G26" s="117"/>
-      <c r="H26" s="118"/>
-      <c r="I26" s="119" t="s">
+      <c r="G26" s="104"/>
+      <c r="H26" s="105"/>
+      <c r="I26" s="106" t="s">
         <v>340</v>
       </c>
-      <c r="J26" s="119"/>
-      <c r="K26" s="120"/>
+      <c r="J26" s="106"/>
+      <c r="K26" s="107"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F27" s="108" t="s">
+      <c r="F27" s="110" t="s">
         <v>341</v>
       </c>
-      <c r="G27" s="109"/>
-      <c r="H27" s="110"/>
-      <c r="I27" s="103" t="s">
+      <c r="G27" s="111"/>
+      <c r="H27" s="112"/>
+      <c r="I27" s="118" t="s">
         <v>342</v>
       </c>
-      <c r="J27" s="103"/>
-      <c r="K27" s="104"/>
+      <c r="J27" s="118"/>
+      <c r="K27" s="119"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F28" s="111" t="s">
+      <c r="F28" s="113" t="s">
         <v>343</v>
       </c>
-      <c r="G28" s="101"/>
-      <c r="H28" s="112"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="114"/>
       <c r="I28" s="83" t="s">
         <v>344</v>
       </c>
       <c r="J28" s="83"/>
-      <c r="K28" s="105"/>
+      <c r="K28" s="120"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F29" s="111" t="s">
+      <c r="F29" s="113" t="s">
         <v>345</v>
       </c>
-      <c r="G29" s="101"/>
-      <c r="H29" s="112"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="114"/>
       <c r="I29" s="83" t="s">
         <v>347</v>
       </c>
       <c r="J29" s="83"/>
-      <c r="K29" s="105"/>
+      <c r="K29" s="120"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F30" s="111" t="s">
+      <c r="F30" s="113" t="s">
         <v>348</v>
       </c>
-      <c r="G30" s="101"/>
-      <c r="H30" s="112"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="114"/>
       <c r="I30" s="83" t="s">
         <v>346</v>
       </c>
       <c r="J30" s="83"/>
-      <c r="K30" s="105"/>
+      <c r="K30" s="120"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F31" s="111" t="s">
+      <c r="F31" s="113" t="s">
         <v>349</v>
       </c>
-      <c r="G31" s="101"/>
-      <c r="H31" s="112"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="114"/>
       <c r="I31" s="83" t="s">
         <v>350</v>
       </c>
       <c r="J31" s="83"/>
-      <c r="K31" s="105"/>
+      <c r="K31" s="120"/>
     </row>
     <row r="32" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F32" s="113" t="s">
+      <c r="F32" s="115" t="s">
         <v>351</v>
       </c>
-      <c r="G32" s="114"/>
-      <c r="H32" s="115"/>
-      <c r="I32" s="106" t="s">
+      <c r="G32" s="116"/>
+      <c r="H32" s="117"/>
+      <c r="I32" s="108" t="s">
         <v>352</v>
       </c>
-      <c r="J32" s="106"/>
-      <c r="K32" s="107"/>
+      <c r="J32" s="108"/>
+      <c r="K32" s="109"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="F25:K25"/>
     <mergeCell ref="I32:K32"/>
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="F28:H28"/>
@@ -6533,6 +7059,12 @@
     <mergeCell ref="I29:K29"/>
     <mergeCell ref="I30:K30"/>
     <mergeCell ref="I31:K31"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="F25:K25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
V3.00.01 - fix(boards): Correction of Warehouse_v2 and Axis_Portal_V2
Correction of the encoder reset in the warehouse v2 board. Additional
modifications to the ACTUATOR_MASK to allow the crane to automatically
align with the shelves. Change to lpf file for Inductive sensor.

Corrections to the documentation of the boards.
</commit_message>
<xml_diff>
--- a/hardware/boards/warehouse_v2/docs/Documentation_WH.xlsx
+++ b/hardware/boards/warehouse_v2/docs/Documentation_WH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\josep\goldi2\hardware\boards\warehouse_v2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11FC5A6-5DE1-4523-BB81-C86557C97A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729D4C0C-33F3-4103-9910-A65FB6F9105A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{658C6C44-180A-4413-9118-4B5F379EEF28}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{658C6C44-180A-4413-9118-4B5F379EEF28}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="410">
   <si>
     <t>Signal Name</t>
   </si>
@@ -1266,6 +1266,24 @@
       </rPr>
       <t>± 10mm). This is done to prevent collisions with the sides of the shelves and other boxes above and below.</t>
     </r>
+  </si>
+  <si>
+    <t>hold_x</t>
+  </si>
+  <si>
+    <t>hold_z</t>
+  </si>
+  <si>
+    <t>enb_y</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>hold_x / hold_z: Disables the movement of the crane when a virtual sensor is detected</t>
+  </si>
+  <si>
+    <t>enb_y: Partially disables the protection system and enables the movement of y motor even when not in the virtual sensor area</t>
   </si>
 </sst>
 </file>
@@ -1437,7 +1455,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="61">
+  <borders count="64">
     <border>
       <left/>
       <right/>
@@ -2175,12 +2193,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2430,6 +2479,51 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3773,7 +3867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8612B84-7723-4382-B2A3-29358A2C76FA}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
@@ -4850,8 +4944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600D60C1-9E46-4611-A95F-ACE45A8F393A}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5250,7 +5344,7 @@
         <v>69</v>
       </c>
       <c r="D21" s="21">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E21" s="62" t="s">
         <v>70</v>
@@ -5954,10 +6048,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:L42"/>
+  <dimension ref="A2:L49"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="B2" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5973,26 +6067,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="132" t="s">
         <v>146</v>
       </c>
-      <c r="B2" s="117"/>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
+      <c r="B2" s="132"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="132"/>
+      <c r="L2" s="132"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="133" t="s">
         <v>147</v>
       </c>
-      <c r="B3" s="118"/>
+      <c r="B3" s="133"/>
       <c r="C3" s="1">
         <v>1</v>
       </c>
@@ -6007,10 +6101,10 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="133" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="118"/>
+      <c r="B4" s="133"/>
       <c r="C4" s="2" t="s">
         <v>402</v>
       </c>
@@ -6025,10 +6119,10 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="133" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="118"/>
+      <c r="B5" s="133"/>
       <c r="C5" s="3" t="s">
         <v>389</v>
       </c>
@@ -6043,34 +6137,34 @@
       <c r="L5" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="119" t="s">
+      <c r="A7" s="134" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="119"/>
-      <c r="C7" s="119"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
-      <c r="J7" s="119"/>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
+      <c r="B7" s="134"/>
+      <c r="C7" s="134"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="134"/>
+      <c r="H7" s="134"/>
+      <c r="I7" s="134"/>
+      <c r="J7" s="134"/>
+      <c r="K7" s="134"/>
+      <c r="L7" s="134"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="119"/>
-      <c r="B8" s="119"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="119"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119"/>
+      <c r="A8" s="134"/>
+      <c r="B8" s="134"/>
+      <c r="C8" s="134"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="134"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="134"/>
+      <c r="I8" s="134"/>
+      <c r="J8" s="134"/>
+      <c r="K8" s="134"/>
+      <c r="L8" s="134"/>
     </row>
     <row r="9" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="13"/>
@@ -6133,9 +6227,15 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="17"/>
+      <c r="H11" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>405</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>404</v>
+      </c>
       <c r="K11" s="17" t="s">
         <v>399</v>
       </c>
@@ -6388,16 +6488,16 @@
       <c r="D19" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E19" s="116" t="s">
+      <c r="E19" s="131" t="s">
         <v>238</v>
       </c>
-      <c r="F19" s="116"/>
-      <c r="G19" s="116"/>
-      <c r="H19" s="116"/>
-      <c r="I19" s="116"/>
-      <c r="J19" s="116"/>
-      <c r="K19" s="116"/>
-      <c r="L19" s="114"/>
+      <c r="F19" s="131"/>
+      <c r="G19" s="131"/>
+      <c r="H19" s="131"/>
+      <c r="I19" s="131"/>
+      <c r="J19" s="131"/>
+      <c r="K19" s="131"/>
+      <c r="L19" s="129"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
@@ -6412,16 +6512,16 @@
       <c r="D20" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E20" s="116" t="s">
+      <c r="E20" s="131" t="s">
         <v>241</v>
       </c>
-      <c r="F20" s="116"/>
-      <c r="G20" s="116"/>
-      <c r="H20" s="116"/>
-      <c r="I20" s="116"/>
-      <c r="J20" s="116"/>
-      <c r="K20" s="116"/>
-      <c r="L20" s="114"/>
+      <c r="F20" s="131"/>
+      <c r="G20" s="131"/>
+      <c r="H20" s="131"/>
+      <c r="I20" s="131"/>
+      <c r="J20" s="131"/>
+      <c r="K20" s="131"/>
+      <c r="L20" s="129"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
@@ -6436,16 +6536,16 @@
       <c r="D21" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E21" s="116" t="s">
+      <c r="E21" s="131" t="s">
         <v>239</v>
       </c>
-      <c r="F21" s="116"/>
-      <c r="G21" s="116"/>
-      <c r="H21" s="116"/>
-      <c r="I21" s="116"/>
-      <c r="J21" s="116"/>
-      <c r="K21" s="116"/>
-      <c r="L21" s="114"/>
+      <c r="F21" s="131"/>
+      <c r="G21" s="131"/>
+      <c r="H21" s="131"/>
+      <c r="I21" s="131"/>
+      <c r="J21" s="131"/>
+      <c r="K21" s="131"/>
+      <c r="L21" s="129"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
@@ -6460,16 +6560,16 @@
       <c r="D22" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E22" s="116" t="s">
+      <c r="E22" s="131" t="s">
         <v>240</v>
       </c>
-      <c r="F22" s="116"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="116"/>
-      <c r="I22" s="116"/>
-      <c r="J22" s="116"/>
-      <c r="K22" s="116"/>
-      <c r="L22" s="114"/>
+      <c r="F22" s="131"/>
+      <c r="G22" s="131"/>
+      <c r="H22" s="131"/>
+      <c r="I22" s="131"/>
+      <c r="J22" s="131"/>
+      <c r="K22" s="131"/>
+      <c r="L22" s="129"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
@@ -6514,16 +6614,16 @@
       <c r="D24" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E24" s="116" t="s">
+      <c r="E24" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="F24" s="116"/>
-      <c r="G24" s="116"/>
-      <c r="H24" s="116"/>
-      <c r="I24" s="116"/>
-      <c r="J24" s="116"/>
-      <c r="K24" s="116"/>
-      <c r="L24" s="114"/>
+      <c r="F24" s="131"/>
+      <c r="G24" s="131"/>
+      <c r="H24" s="131"/>
+      <c r="I24" s="131"/>
+      <c r="J24" s="131"/>
+      <c r="K24" s="131"/>
+      <c r="L24" s="129"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
@@ -6538,16 +6638,16 @@
       <c r="D25" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E25" s="114" t="s">
+      <c r="E25" s="129" t="s">
         <v>264</v>
       </c>
-      <c r="F25" s="115"/>
-      <c r="G25" s="115"/>
-      <c r="H25" s="115"/>
-      <c r="I25" s="115"/>
-      <c r="J25" s="115"/>
-      <c r="K25" s="115"/>
-      <c r="L25" s="115"/>
+      <c r="F25" s="130"/>
+      <c r="G25" s="130"/>
+      <c r="H25" s="130"/>
+      <c r="I25" s="130"/>
+      <c r="J25" s="130"/>
+      <c r="K25" s="130"/>
+      <c r="L25" s="130"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
@@ -6562,16 +6662,16 @@
       <c r="D26" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="E26" s="116" t="s">
+      <c r="E26" s="131" t="s">
         <v>243</v>
       </c>
-      <c r="F26" s="116"/>
-      <c r="G26" s="116"/>
-      <c r="H26" s="116"/>
-      <c r="I26" s="116"/>
-      <c r="J26" s="116"/>
-      <c r="K26" s="116"/>
-      <c r="L26" s="114"/>
+      <c r="F26" s="131"/>
+      <c r="G26" s="131"/>
+      <c r="H26" s="131"/>
+      <c r="I26" s="131"/>
+      <c r="J26" s="131"/>
+      <c r="K26" s="131"/>
+      <c r="L26" s="129"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
@@ -6586,16 +6686,16 @@
       <c r="D27" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E27" s="116" t="s">
+      <c r="E27" s="131" t="s">
         <v>244</v>
       </c>
-      <c r="F27" s="116"/>
-      <c r="G27" s="116"/>
-      <c r="H27" s="116"/>
-      <c r="I27" s="116"/>
-      <c r="J27" s="116"/>
-      <c r="K27" s="116"/>
-      <c r="L27" s="114"/>
+      <c r="F27" s="131"/>
+      <c r="G27" s="131"/>
+      <c r="H27" s="131"/>
+      <c r="I27" s="131"/>
+      <c r="J27" s="131"/>
+      <c r="K27" s="131"/>
+      <c r="L27" s="129"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
@@ -6610,16 +6710,16 @@
       <c r="D28" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E28" s="114" t="s">
+      <c r="E28" s="129" t="s">
         <v>298</v>
       </c>
-      <c r="F28" s="115"/>
-      <c r="G28" s="115"/>
-      <c r="H28" s="115"/>
-      <c r="I28" s="115"/>
-      <c r="J28" s="115"/>
-      <c r="K28" s="115"/>
-      <c r="L28" s="115"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="130"/>
+      <c r="H28" s="130"/>
+      <c r="I28" s="130"/>
+      <c r="J28" s="130"/>
+      <c r="K28" s="130"/>
+      <c r="L28" s="130"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
@@ -6660,16 +6760,16 @@
       <c r="D30" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E30" s="116" t="s">
+      <c r="E30" s="131" t="s">
         <v>245</v>
       </c>
-      <c r="F30" s="116"/>
-      <c r="G30" s="116"/>
-      <c r="H30" s="116"/>
-      <c r="I30" s="116"/>
-      <c r="J30" s="116"/>
-      <c r="K30" s="116"/>
-      <c r="L30" s="114"/>
+      <c r="F30" s="131"/>
+      <c r="G30" s="131"/>
+      <c r="H30" s="131"/>
+      <c r="I30" s="131"/>
+      <c r="J30" s="131"/>
+      <c r="K30" s="131"/>
+      <c r="L30" s="129"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
@@ -6714,16 +6814,16 @@
       <c r="D32" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E32" s="116" t="s">
+      <c r="E32" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="F32" s="116"/>
-      <c r="G32" s="116"/>
-      <c r="H32" s="116"/>
-      <c r="I32" s="116"/>
-      <c r="J32" s="116"/>
-      <c r="K32" s="116"/>
-      <c r="L32" s="114"/>
+      <c r="F32" s="131"/>
+      <c r="G32" s="131"/>
+      <c r="H32" s="131"/>
+      <c r="I32" s="131"/>
+      <c r="J32" s="131"/>
+      <c r="K32" s="131"/>
+      <c r="L32" s="129"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
@@ -6738,16 +6838,16 @@
       <c r="D33" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E33" s="116" t="s">
+      <c r="E33" s="131" t="s">
         <v>264</v>
       </c>
-      <c r="F33" s="116"/>
-      <c r="G33" s="116"/>
-      <c r="H33" s="116"/>
-      <c r="I33" s="116"/>
-      <c r="J33" s="116"/>
-      <c r="K33" s="116"/>
-      <c r="L33" s="114"/>
+      <c r="F33" s="131"/>
+      <c r="G33" s="131"/>
+      <c r="H33" s="131"/>
+      <c r="I33" s="131"/>
+      <c r="J33" s="131"/>
+      <c r="K33" s="131"/>
+      <c r="L33" s="129"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
@@ -6762,16 +6862,16 @@
       <c r="D34" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="E34" s="116" t="s">
+      <c r="E34" s="131" t="s">
         <v>243</v>
       </c>
-      <c r="F34" s="116"/>
-      <c r="G34" s="116"/>
-      <c r="H34" s="116"/>
-      <c r="I34" s="116"/>
-      <c r="J34" s="116"/>
-      <c r="K34" s="116"/>
-      <c r="L34" s="114"/>
+      <c r="F34" s="131"/>
+      <c r="G34" s="131"/>
+      <c r="H34" s="131"/>
+      <c r="I34" s="131"/>
+      <c r="J34" s="131"/>
+      <c r="K34" s="131"/>
+      <c r="L34" s="129"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
@@ -6786,16 +6886,16 @@
       <c r="D35" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E35" s="116" t="s">
+      <c r="E35" s="131" t="s">
         <v>244</v>
       </c>
-      <c r="F35" s="116"/>
-      <c r="G35" s="116"/>
-      <c r="H35" s="116"/>
-      <c r="I35" s="116"/>
-      <c r="J35" s="116"/>
-      <c r="K35" s="116"/>
-      <c r="L35" s="114"/>
+      <c r="F35" s="131"/>
+      <c r="G35" s="131"/>
+      <c r="H35" s="131"/>
+      <c r="I35" s="131"/>
+      <c r="J35" s="131"/>
+      <c r="K35" s="131"/>
+      <c r="L35" s="129"/>
     </row>
     <row r="36" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
@@ -6810,16 +6910,16 @@
       <c r="D36" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="E36" s="114" t="s">
+      <c r="E36" s="129" t="s">
         <v>298</v>
       </c>
-      <c r="F36" s="115"/>
-      <c r="G36" s="115"/>
-      <c r="H36" s="115"/>
-      <c r="I36" s="115"/>
-      <c r="J36" s="115"/>
-      <c r="K36" s="115"/>
-      <c r="L36" s="115"/>
+      <c r="F36" s="130"/>
+      <c r="G36" s="130"/>
+      <c r="H36" s="130"/>
+      <c r="I36" s="130"/>
+      <c r="J36" s="130"/>
+      <c r="K36" s="130"/>
+      <c r="L36" s="130"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -6840,16 +6940,16 @@
       <c r="F37" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="G37" s="122" t="s">
+      <c r="G37" s="137" t="s">
         <v>254</v>
       </c>
-      <c r="H37" s="122"/>
-      <c r="I37" s="122"/>
-      <c r="J37" s="122" t="s">
+      <c r="H37" s="137"/>
+      <c r="I37" s="137"/>
+      <c r="J37" s="137" t="s">
         <v>255</v>
       </c>
-      <c r="K37" s="122"/>
-      <c r="L37" s="123"/>
+      <c r="K37" s="137"/>
+      <c r="L37" s="138"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
@@ -6870,16 +6970,16 @@
       <c r="F38" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="G38" s="122" t="s">
+      <c r="G38" s="137" t="s">
         <v>254</v>
       </c>
-      <c r="H38" s="122"/>
-      <c r="I38" s="122"/>
-      <c r="J38" s="122" t="s">
+      <c r="H38" s="137"/>
+      <c r="I38" s="137"/>
+      <c r="J38" s="137" t="s">
         <v>255</v>
       </c>
-      <c r="K38" s="122"/>
-      <c r="L38" s="123"/>
+      <c r="K38" s="137"/>
+      <c r="L38" s="138"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
@@ -6900,16 +7000,16 @@
       <c r="F39" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="G39" s="122" t="s">
+      <c r="G39" s="137" t="s">
         <v>254</v>
       </c>
-      <c r="H39" s="122"/>
-      <c r="I39" s="122"/>
-      <c r="J39" s="122" t="s">
+      <c r="H39" s="137"/>
+      <c r="I39" s="137"/>
+      <c r="J39" s="137" t="s">
         <v>255</v>
       </c>
-      <c r="K39" s="122"/>
-      <c r="L39" s="123"/>
+      <c r="K39" s="137"/>
+      <c r="L39" s="138"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
@@ -6930,16 +7030,16 @@
       <c r="F40" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="G40" s="122" t="s">
+      <c r="G40" s="137" t="s">
         <v>254</v>
       </c>
-      <c r="H40" s="122"/>
-      <c r="I40" s="122"/>
-      <c r="J40" s="122" t="s">
+      <c r="H40" s="137"/>
+      <c r="I40" s="137"/>
+      <c r="J40" s="137" t="s">
         <v>255</v>
       </c>
-      <c r="K40" s="122"/>
-      <c r="L40" s="123"/>
+      <c r="K40" s="137"/>
+      <c r="L40" s="138"/>
     </row>
     <row r="41" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="25" t="s">
@@ -6960,30 +7060,117 @@
       <c r="F41" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="G41" s="120" t="s">
+      <c r="G41" s="135" t="s">
         <v>254</v>
       </c>
-      <c r="H41" s="120"/>
-      <c r="I41" s="120"/>
-      <c r="J41" s="120" t="s">
+      <c r="H41" s="135"/>
+      <c r="I41" s="135"/>
+      <c r="J41" s="135" t="s">
         <v>255</v>
       </c>
-      <c r="K41" s="120"/>
-      <c r="L41" s="121"/>
+      <c r="K41" s="135"/>
+      <c r="L41" s="136"/>
     </row>
     <row r="42" spans="1:12" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B42" s="29"/>
       <c r="C42" s="29"/>
       <c r="F42" s="29"/>
     </row>
+    <row r="44" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="114" t="s">
+        <v>407</v>
+      </c>
+      <c r="D45" s="115"/>
+      <c r="E45" s="115"/>
+      <c r="F45" s="115"/>
+      <c r="G45" s="115"/>
+      <c r="H45" s="115"/>
+      <c r="I45" s="115"/>
+      <c r="J45" s="115"/>
+      <c r="K45" s="115"/>
+      <c r="L45" s="116"/>
+    </row>
+    <row r="46" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="123" t="s">
+        <v>408</v>
+      </c>
+      <c r="D46" s="124"/>
+      <c r="E46" s="124"/>
+      <c r="F46" s="124"/>
+      <c r="G46" s="124"/>
+      <c r="H46" s="124"/>
+      <c r="I46" s="124"/>
+      <c r="J46" s="124"/>
+      <c r="K46" s="124"/>
+      <c r="L46" s="125"/>
+    </row>
+    <row r="47" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="126"/>
+      <c r="D47" s="127"/>
+      <c r="E47" s="127"/>
+      <c r="F47" s="127"/>
+      <c r="G47" s="127"/>
+      <c r="H47" s="127"/>
+      <c r="I47" s="127"/>
+      <c r="J47" s="127"/>
+      <c r="K47" s="127"/>
+      <c r="L47" s="128"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C48" s="117" t="s">
+        <v>409</v>
+      </c>
+      <c r="D48" s="118"/>
+      <c r="E48" s="118"/>
+      <c r="F48" s="118"/>
+      <c r="G48" s="118"/>
+      <c r="H48" s="118"/>
+      <c r="I48" s="118"/>
+      <c r="J48" s="118"/>
+      <c r="K48" s="118"/>
+      <c r="L48" s="119"/>
+    </row>
+    <row r="49" spans="3:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="120"/>
+      <c r="D49" s="121"/>
+      <c r="E49" s="121"/>
+      <c r="F49" s="121"/>
+      <c r="G49" s="121"/>
+      <c r="H49" s="121"/>
+      <c r="I49" s="121"/>
+      <c r="J49" s="121"/>
+      <c r="K49" s="121"/>
+      <c r="L49" s="122"/>
+    </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="33">
+    <mergeCell ref="J39:L39"/>
     <mergeCell ref="E32:L32"/>
     <mergeCell ref="E34:L34"/>
     <mergeCell ref="E35:L35"/>
     <mergeCell ref="G37:I37"/>
     <mergeCell ref="J37:L37"/>
     <mergeCell ref="E36:L36"/>
+    <mergeCell ref="E19:L19"/>
+    <mergeCell ref="E20:L20"/>
+    <mergeCell ref="E21:L21"/>
+    <mergeCell ref="E22:L22"/>
+    <mergeCell ref="E24:L24"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:L8"/>
+    <mergeCell ref="C45:L45"/>
+    <mergeCell ref="C48:L49"/>
+    <mergeCell ref="C46:L47"/>
+    <mergeCell ref="E25:L25"/>
+    <mergeCell ref="E33:L33"/>
+    <mergeCell ref="E26:L26"/>
+    <mergeCell ref="E27:L27"/>
+    <mergeCell ref="E30:L30"/>
+    <mergeCell ref="E28:L28"/>
     <mergeCell ref="G41:I41"/>
     <mergeCell ref="J41:L41"/>
     <mergeCell ref="G38:I38"/>
@@ -6991,27 +7178,10 @@
     <mergeCell ref="G40:I40"/>
     <mergeCell ref="J40:L40"/>
     <mergeCell ref="G39:I39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="E25:L25"/>
-    <mergeCell ref="E33:L33"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:L8"/>
-    <mergeCell ref="E19:L19"/>
-    <mergeCell ref="E20:L20"/>
-    <mergeCell ref="E21:L21"/>
-    <mergeCell ref="E22:L22"/>
-    <mergeCell ref="E24:L24"/>
-    <mergeCell ref="E26:L26"/>
-    <mergeCell ref="E27:L27"/>
-    <mergeCell ref="E30:L30"/>
-    <mergeCell ref="E28:L28"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="83" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="72" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;P</oddFooter>
   </headerFooter>
@@ -7057,25 +7227,25 @@
       <c r="A4" s="67" t="s">
         <v>271</v>
       </c>
-      <c r="B4" s="125" t="s">
+      <c r="B4" s="140" t="s">
         <v>272</v>
       </c>
-      <c r="C4" s="126"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
-      <c r="H4" s="126"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="126"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="141"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="141"/>
+      <c r="G4" s="141"/>
+      <c r="H4" s="141"/>
+      <c r="I4" s="141"/>
+      <c r="J4" s="141"/>
+      <c r="K4" s="141"/>
+      <c r="L4" s="141"/>
     </row>
     <row r="5" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="68" t="s">
         <v>237</v>
       </c>
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="139" t="s">
         <v>286</v>
       </c>
       <c r="C5" s="89"/>
@@ -7093,7 +7263,7 @@
       <c r="A6" s="69" t="s">
         <v>273</v>
       </c>
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="139" t="s">
         <v>285</v>
       </c>
       <c r="C6" s="89"/>
@@ -7111,7 +7281,7 @@
       <c r="A7" s="69" t="s">
         <v>274</v>
       </c>
-      <c r="B7" s="124" t="s">
+      <c r="B7" s="139" t="s">
         <v>287</v>
       </c>
       <c r="C7" s="89"/>
@@ -7129,7 +7299,7 @@
       <c r="A8" s="69" t="s">
         <v>275</v>
       </c>
-      <c r="B8" s="124" t="s">
+      <c r="B8" s="139" t="s">
         <v>297</v>
       </c>
       <c r="C8" s="89"/>
@@ -7147,7 +7317,7 @@
       <c r="A9" s="69" t="s">
         <v>276</v>
       </c>
-      <c r="B9" s="124" t="s">
+      <c r="B9" s="139" t="s">
         <v>296</v>
       </c>
       <c r="C9" s="89"/>
@@ -7165,7 +7335,7 @@
       <c r="A10" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="B10" s="124" t="s">
+      <c r="B10" s="139" t="s">
         <v>295</v>
       </c>
       <c r="C10" s="89"/>
@@ -7183,7 +7353,7 @@
       <c r="A11" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="B11" s="124" t="s">
+      <c r="B11" s="139" t="s">
         <v>294</v>
       </c>
       <c r="C11" s="89"/>
@@ -7201,7 +7371,7 @@
       <c r="A12" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="B12" s="124" t="s">
+      <c r="B12" s="139" t="s">
         <v>293</v>
       </c>
       <c r="C12" s="89"/>
@@ -7219,7 +7389,7 @@
       <c r="A13" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="B13" s="124" t="s">
+      <c r="B13" s="139" t="s">
         <v>292</v>
       </c>
       <c r="C13" s="89"/>
@@ -7237,7 +7407,7 @@
       <c r="A14" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="B14" s="124" t="s">
+      <c r="B14" s="139" t="s">
         <v>291</v>
       </c>
       <c r="C14" s="89"/>
@@ -7255,7 +7425,7 @@
       <c r="A15" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="B15" s="124" t="s">
+      <c r="B15" s="139" t="s">
         <v>290</v>
       </c>
       <c r="C15" s="89"/>
@@ -7273,7 +7443,7 @@
       <c r="A16" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="B16" s="124" t="s">
+      <c r="B16" s="139" t="s">
         <v>289</v>
       </c>
       <c r="C16" s="89"/>
@@ -7291,7 +7461,7 @@
       <c r="A17" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="B17" s="124" t="s">
+      <c r="B17" s="139" t="s">
         <v>288</v>
       </c>
       <c r="C17" s="89"/>
@@ -7378,19 +7548,19 @@
       <c r="M2" s="90"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="128"/>
-      <c r="B3" s="128"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
+      <c r="A3" s="143"/>
+      <c r="B3" s="143"/>
+      <c r="C3" s="143"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="143"/>
+      <c r="F3" s="143"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="143"/>
+      <c r="I3" s="143"/>
+      <c r="J3" s="143"/>
+      <c r="K3" s="143"/>
+      <c r="L3" s="143"/>
+      <c r="M3" s="143"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="84" t="s">
@@ -7536,19 +7706,19 @@
       <c r="M12" s="91"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="127"/>
-      <c r="B13" s="127"/>
-      <c r="C13" s="127"/>
-      <c r="D13" s="127"/>
-      <c r="E13" s="127"/>
-      <c r="F13" s="127"/>
-      <c r="G13" s="127"/>
-      <c r="H13" s="127"/>
-      <c r="I13" s="127"/>
-      <c r="J13" s="127"/>
-      <c r="K13" s="127"/>
-      <c r="L13" s="127"/>
-      <c r="M13" s="127"/>
+      <c r="A13" s="142"/>
+      <c r="B13" s="142"/>
+      <c r="C13" s="142"/>
+      <c r="D13" s="142"/>
+      <c r="E13" s="142"/>
+      <c r="F13" s="142"/>
+      <c r="G13" s="142"/>
+      <c r="H13" s="142"/>
+      <c r="I13" s="142"/>
+      <c r="J13" s="142"/>
+      <c r="K13" s="142"/>
+      <c r="L13" s="142"/>
+      <c r="M13" s="142"/>
     </row>
     <row r="14" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="91" t="s">
@@ -7628,19 +7798,19 @@
       <c r="M18" s="91"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="127"/>
-      <c r="B19" s="127"/>
-      <c r="C19" s="127"/>
-      <c r="D19" s="127"/>
-      <c r="E19" s="127"/>
-      <c r="F19" s="127"/>
-      <c r="G19" s="127"/>
-      <c r="H19" s="127"/>
-      <c r="I19" s="127"/>
-      <c r="J19" s="127"/>
-      <c r="K19" s="127"/>
-      <c r="L19" s="127"/>
-      <c r="M19" s="127"/>
+      <c r="A19" s="142"/>
+      <c r="B19" s="142"/>
+      <c r="C19" s="142"/>
+      <c r="D19" s="142"/>
+      <c r="E19" s="142"/>
+      <c r="F19" s="142"/>
+      <c r="G19" s="142"/>
+      <c r="H19" s="142"/>
+      <c r="I19" s="142"/>
+      <c r="J19" s="142"/>
+      <c r="K19" s="142"/>
+      <c r="L19" s="142"/>
+      <c r="M19" s="142"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="91" t="s">
@@ -8151,101 +8321,101 @@
       </c>
     </row>
     <row r="25" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F25" s="129" t="s">
+      <c r="F25" s="144" t="s">
         <v>310</v>
       </c>
-      <c r="G25" s="130"/>
-      <c r="H25" s="130"/>
-      <c r="I25" s="130"/>
-      <c r="J25" s="130"/>
-      <c r="K25" s="131"/>
+      <c r="G25" s="145"/>
+      <c r="H25" s="145"/>
+      <c r="I25" s="145"/>
+      <c r="J25" s="145"/>
+      <c r="K25" s="146"/>
     </row>
     <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>309</v>
       </c>
-      <c r="F26" s="129" t="s">
+      <c r="F26" s="144" t="s">
         <v>311</v>
       </c>
-      <c r="G26" s="130"/>
-      <c r="H26" s="131"/>
-      <c r="I26" s="132" t="s">
+      <c r="G26" s="145"/>
+      <c r="H26" s="146"/>
+      <c r="I26" s="147" t="s">
         <v>312</v>
       </c>
-      <c r="J26" s="132"/>
-      <c r="K26" s="133"/>
+      <c r="J26" s="147"/>
+      <c r="K26" s="148"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F27" s="136" t="s">
+      <c r="F27" s="151" t="s">
         <v>313</v>
       </c>
-      <c r="G27" s="137"/>
-      <c r="H27" s="138"/>
-      <c r="I27" s="145" t="s">
+      <c r="G27" s="152"/>
+      <c r="H27" s="153"/>
+      <c r="I27" s="160" t="s">
         <v>314</v>
       </c>
-      <c r="J27" s="145"/>
-      <c r="K27" s="146"/>
+      <c r="J27" s="160"/>
+      <c r="K27" s="161"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F28" s="139" t="s">
+      <c r="F28" s="154" t="s">
         <v>315</v>
       </c>
-      <c r="G28" s="140"/>
-      <c r="H28" s="141"/>
-      <c r="I28" s="147" t="s">
+      <c r="G28" s="155"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="162" t="s">
         <v>316</v>
       </c>
-      <c r="J28" s="147"/>
-      <c r="K28" s="148"/>
+      <c r="J28" s="162"/>
+      <c r="K28" s="163"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F29" s="139" t="s">
+      <c r="F29" s="154" t="s">
         <v>317</v>
       </c>
-      <c r="G29" s="140"/>
-      <c r="H29" s="141"/>
-      <c r="I29" s="147" t="s">
+      <c r="G29" s="155"/>
+      <c r="H29" s="156"/>
+      <c r="I29" s="162" t="s">
         <v>319</v>
       </c>
-      <c r="J29" s="147"/>
-      <c r="K29" s="148"/>
+      <c r="J29" s="162"/>
+      <c r="K29" s="163"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F30" s="139" t="s">
+      <c r="F30" s="154" t="s">
         <v>320</v>
       </c>
-      <c r="G30" s="140"/>
-      <c r="H30" s="141"/>
-      <c r="I30" s="147" t="s">
+      <c r="G30" s="155"/>
+      <c r="H30" s="156"/>
+      <c r="I30" s="162" t="s">
         <v>318</v>
       </c>
-      <c r="J30" s="147"/>
-      <c r="K30" s="148"/>
+      <c r="J30" s="162"/>
+      <c r="K30" s="163"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="F31" s="139" t="s">
+      <c r="F31" s="154" t="s">
         <v>321</v>
       </c>
-      <c r="G31" s="140"/>
-      <c r="H31" s="141"/>
-      <c r="I31" s="147" t="s">
+      <c r="G31" s="155"/>
+      <c r="H31" s="156"/>
+      <c r="I31" s="162" t="s">
         <v>322</v>
       </c>
-      <c r="J31" s="147"/>
-      <c r="K31" s="148"/>
+      <c r="J31" s="162"/>
+      <c r="K31" s="163"/>
     </row>
     <row r="32" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F32" s="142" t="s">
+      <c r="F32" s="157" t="s">
         <v>323</v>
       </c>
-      <c r="G32" s="143"/>
-      <c r="H32" s="144"/>
-      <c r="I32" s="134" t="s">
+      <c r="G32" s="158"/>
+      <c r="H32" s="159"/>
+      <c r="I32" s="149" t="s">
         <v>324</v>
       </c>
-      <c r="J32" s="134"/>
-      <c r="K32" s="135"/>
+      <c r="J32" s="149"/>
+      <c r="K32" s="150"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -8291,16 +8461,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="149"/>
-      <c r="B1" s="149"/>
-      <c r="C1" s="149"/>
-      <c r="D1" s="149"/>
-      <c r="E1" s="149"/>
-      <c r="F1" s="149"/>
-      <c r="G1" s="149"/>
-      <c r="H1" s="149"/>
-      <c r="I1" s="149"/>
-      <c r="J1" s="149"/>
+      <c r="A1" s="164"/>
+      <c r="B1" s="164"/>
+      <c r="C1" s="164"/>
+      <c r="D1" s="164"/>
+      <c r="E1" s="164"/>
+      <c r="F1" s="164"/>
+      <c r="G1" s="164"/>
+      <c r="H1" s="164"/>
+      <c r="I1" s="164"/>
+      <c r="J1" s="164"/>
     </row>
     <row r="2" spans="1:10" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="90" t="s">
@@ -8317,16 +8487,16 @@
       <c r="J2" s="90"/>
     </row>
     <row r="3" spans="1:10" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="150"/>
-      <c r="B3" s="150"/>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="150"/>
-      <c r="H3" s="150"/>
-      <c r="I3" s="150"/>
-      <c r="J3" s="150"/>
+      <c r="A3" s="165"/>
+      <c r="B3" s="165"/>
+      <c r="C3" s="165"/>
+      <c r="D3" s="165"/>
+      <c r="E3" s="165"/>
+      <c r="F3" s="165"/>
+      <c r="G3" s="165"/>
+      <c r="H3" s="165"/>
+      <c r="I3" s="165"/>
+      <c r="J3" s="165"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="84" t="s">
@@ -8810,10 +8980,10 @@
       <c r="J56" s="91"/>
     </row>
     <row r="57" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="151" t="s">
+      <c r="A57" s="166" t="s">
         <v>375</v>
       </c>
-      <c r="B57" s="151"/>
+      <c r="B57" s="166"/>
       <c r="C57" s="91" t="s">
         <v>379</v>
       </c>
@@ -8826,10 +8996,10 @@
       <c r="J57" s="91"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="151" t="s">
+      <c r="A58" s="166" t="s">
         <v>376</v>
       </c>
-      <c r="B58" s="151"/>
+      <c r="B58" s="166"/>
       <c r="C58" s="91" t="s">
         <v>377</v>
       </c>
@@ -8842,10 +9012,10 @@
       <c r="J58" s="91"/>
     </row>
     <row r="59" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="151" t="s">
+      <c r="A59" s="166" t="s">
         <v>378</v>
       </c>
-      <c r="B59" s="151"/>
+      <c r="B59" s="166"/>
       <c r="C59" s="91" t="s">
         <v>380</v>
       </c>
@@ -8858,8 +9028,8 @@
       <c r="J59" s="91"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="151"/>
-      <c r="B60" s="151"/>
+      <c r="A60" s="166"/>
+      <c r="B60" s="166"/>
       <c r="C60" s="91"/>
       <c r="D60" s="91"/>
       <c r="E60" s="91"/>

</xml_diff>